<commit_message>
Chuyen De Phat Trien Ung Dung 2 - TDC - 2024 Tuan: 5 Ngay: 15/10/2024 De tai: Quan ly sieu thi Nhom: 2 Chau Nhat Tai Nguyen Quoc Luong Le Van Toan
Noi dung cong viec:
- [x] Updated file .mdf
- [x] Added QLST_Scripts.sql

/* Committed? */
- [x] Yes/No

/* Note */
</commit_message>
<xml_diff>
--- a/PTUD/CDUD - 2/files/Nhom2 - CDUD2 - Sprints.xlsx
+++ b/PTUD/CDUD - 2/files/Nhom2 - CDUD2 - Sprints.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STUDY\Chuyen-De-Phat-Trien-Ung-Dung---TDC---2024\PTUD\CDUD - 2\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\NhatTaiC\Chuyen-De-Phat-Trien-Ung-Dung---TDC---2024\PTUD\CDUD - 2\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F0FAB9-3859-4917-86AF-37DF7DDE88EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54BE2532-2A39-4111-960A-EE3A08F33B4B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -483,27 +483,6 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -516,14 +495,41 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -533,12 +539,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -823,7 +823,7 @@
   <dimension ref="G8:O45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11:O15"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -840,17 +840,17 @@
   </cols>
   <sheetData>
     <row r="8" spans="7:15" ht="22.5" x14ac:dyDescent="0.6">
-      <c r="G8" s="18" t="s">
+      <c r="G8" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="22"/>
     </row>
     <row r="10" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
       <c r="G10" s="2" t="s">
@@ -882,16 +882,16 @@
       </c>
     </row>
     <row r="11" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G11" s="12">
+      <c r="G11" s="21">
         <v>1</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="H11" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="I11" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="J11" s="12">
+      <c r="J11" s="21">
         <v>5</v>
       </c>
       <c r="K11" s="1">
@@ -900,83 +900,83 @@
       <c r="L11" s="6">
         <v>45579</v>
       </c>
-      <c r="M11" s="15" t="s">
+      <c r="M11" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="N11" s="19">
+      <c r="N11" s="12">
         <v>15</v>
       </c>
-      <c r="O11" s="15" t="s">
+      <c r="O11" s="16" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="12" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="12"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="21"/>
       <c r="K12" s="1">
         <v>3</v>
       </c>
       <c r="L12" s="6">
         <v>45580</v>
       </c>
-      <c r="M12" s="16"/>
-      <c r="N12" s="20"/>
-      <c r="O12" s="16"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="17"/>
     </row>
     <row r="13" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="12"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="21"/>
       <c r="K13" s="1">
         <v>4</v>
       </c>
       <c r="L13" s="6">
         <v>45581</v>
       </c>
-      <c r="M13" s="16"/>
-      <c r="N13" s="20"/>
-      <c r="O13" s="16"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="17"/>
     </row>
     <row r="14" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="12"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="21"/>
       <c r="K14" s="1">
         <v>5</v>
       </c>
       <c r="L14" s="6">
         <v>45582</v>
       </c>
-      <c r="M14" s="16"/>
-      <c r="N14" s="20"/>
-      <c r="O14" s="16"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="17"/>
     </row>
     <row r="15" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="12"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="21"/>
       <c r="K15" s="1">
         <v>6</v>
       </c>
       <c r="L15" s="6">
         <v>45583</v>
       </c>
-      <c r="M15" s="17"/>
-      <c r="N15" s="21"/>
-      <c r="O15" s="17"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="18"/>
     </row>
     <row r="16" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="13" t="s">
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="J16" s="12">
+      <c r="J16" s="21">
         <v>6</v>
       </c>
       <c r="K16" s="1">
@@ -985,87 +985,87 @@
       <c r="L16" s="6">
         <v>45586</v>
       </c>
-      <c r="M16" s="13" t="s">
+      <c r="M16" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="N16" s="19">
+      <c r="N16" s="12">
         <v>15</v>
       </c>
-      <c r="O16" s="15" t="s">
+      <c r="O16" s="16" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="17" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="12"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="21"/>
       <c r="K17" s="1">
         <v>3</v>
       </c>
       <c r="L17" s="6">
         <v>45587</v>
       </c>
-      <c r="M17" s="14"/>
-      <c r="N17" s="20"/>
-      <c r="O17" s="16"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="17"/>
     </row>
     <row r="18" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="12"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="21"/>
       <c r="K18" s="1">
         <v>4</v>
       </c>
       <c r="L18" s="6">
         <v>45588</v>
       </c>
-      <c r="M18" s="14"/>
-      <c r="N18" s="20"/>
-      <c r="O18" s="16"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="17"/>
     </row>
     <row r="19" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="12"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="21"/>
       <c r="K19" s="1">
         <v>5</v>
       </c>
       <c r="L19" s="6">
         <v>45589</v>
       </c>
-      <c r="M19" s="14"/>
-      <c r="N19" s="20"/>
-      <c r="O19" s="16"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="17"/>
     </row>
     <row r="20" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="12"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="21"/>
       <c r="K20" s="1">
         <v>6</v>
       </c>
       <c r="L20" s="11">
         <v>45590</v>
       </c>
-      <c r="M20" s="14"/>
-      <c r="N20" s="21"/>
-      <c r="O20" s="17"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="18"/>
     </row>
     <row r="21" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G21" s="12">
+      <c r="G21" s="21">
         <v>2</v>
       </c>
-      <c r="H21" s="12" t="s">
+      <c r="H21" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="I21" s="13" t="s">
+      <c r="I21" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="J21" s="12">
+      <c r="J21" s="21">
         <v>7</v>
       </c>
       <c r="K21" s="1">
@@ -1074,83 +1074,83 @@
       <c r="L21" s="6">
         <v>45593</v>
       </c>
-      <c r="M21" s="13" t="s">
+      <c r="M21" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="N21" s="19">
+      <c r="N21" s="12">
         <v>15</v>
       </c>
-      <c r="O21" s="15" t="s">
+      <c r="O21" s="16" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="22" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="12"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="21"/>
       <c r="K22" s="1">
         <v>3</v>
       </c>
       <c r="L22" s="6">
         <v>45594</v>
       </c>
-      <c r="M22" s="14"/>
-      <c r="N22" s="20"/>
-      <c r="O22" s="16"/>
+      <c r="M22" s="20"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="17"/>
     </row>
     <row r="23" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="12"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="21"/>
       <c r="K23" s="1">
         <v>4</v>
       </c>
       <c r="L23" s="6">
         <v>45595</v>
       </c>
-      <c r="M23" s="14"/>
-      <c r="N23" s="20"/>
-      <c r="O23" s="16"/>
+      <c r="M23" s="20"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="17"/>
     </row>
     <row r="24" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="12"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="21"/>
       <c r="K24" s="1">
         <v>5</v>
       </c>
       <c r="L24" s="6">
         <v>45596</v>
       </c>
-      <c r="M24" s="14"/>
-      <c r="N24" s="20"/>
-      <c r="O24" s="16"/>
+      <c r="M24" s="20"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="17"/>
     </row>
     <row r="25" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="12"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="21"/>
       <c r="K25" s="1">
         <v>6</v>
       </c>
       <c r="L25" s="6">
         <v>45597</v>
       </c>
-      <c r="M25" s="14"/>
-      <c r="N25" s="21"/>
-      <c r="O25" s="17"/>
+      <c r="M25" s="20"/>
+      <c r="N25" s="14"/>
+      <c r="O25" s="18"/>
     </row>
     <row r="26" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="13" t="s">
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="J26" s="12">
+      <c r="J26" s="21">
         <v>8</v>
       </c>
       <c r="K26" s="1">
@@ -1159,87 +1159,87 @@
       <c r="L26" s="6">
         <v>45600</v>
       </c>
-      <c r="M26" s="13" t="s">
+      <c r="M26" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="N26" s="19">
+      <c r="N26" s="12">
         <v>15</v>
       </c>
-      <c r="O26" s="15" t="s">
+      <c r="O26" s="16" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="27" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="12"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="21"/>
       <c r="K27" s="1">
         <v>3</v>
       </c>
       <c r="L27" s="6">
         <v>45601</v>
       </c>
-      <c r="M27" s="14"/>
-      <c r="N27" s="20"/>
-      <c r="O27" s="16"/>
+      <c r="M27" s="20"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="17"/>
     </row>
     <row r="28" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="12"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="21"/>
       <c r="K28" s="1">
         <v>4</v>
       </c>
       <c r="L28" s="6">
         <v>45602</v>
       </c>
-      <c r="M28" s="14"/>
-      <c r="N28" s="20"/>
-      <c r="O28" s="16"/>
+      <c r="M28" s="20"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="17"/>
     </row>
     <row r="29" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="12"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="21"/>
       <c r="K29" s="1">
         <v>5</v>
       </c>
       <c r="L29" s="6">
         <v>45603</v>
       </c>
-      <c r="M29" s="14"/>
-      <c r="N29" s="20"/>
-      <c r="O29" s="16"/>
+      <c r="M29" s="20"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="17"/>
     </row>
     <row r="30" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="12"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="21"/>
       <c r="K30" s="1">
         <v>6</v>
       </c>
       <c r="L30" s="6">
         <v>45604</v>
       </c>
-      <c r="M30" s="14"/>
-      <c r="N30" s="21"/>
-      <c r="O30" s="17"/>
+      <c r="M30" s="20"/>
+      <c r="N30" s="14"/>
+      <c r="O30" s="18"/>
     </row>
     <row r="31" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G31" s="12">
+      <c r="G31" s="21">
         <v>3</v>
       </c>
-      <c r="H31" s="12" t="s">
+      <c r="H31" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="I31" s="15" t="s">
+      <c r="I31" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="J31" s="12">
+      <c r="J31" s="21">
         <v>9</v>
       </c>
       <c r="K31" s="1">
@@ -1248,83 +1248,83 @@
       <c r="L31" s="6">
         <v>45607</v>
       </c>
-      <c r="M31" s="15" t="s">
+      <c r="M31" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="N31" s="19">
+      <c r="N31" s="12">
         <v>15</v>
       </c>
-      <c r="O31" s="22" t="s">
+      <c r="O31" s="15" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="32" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
-      <c r="I32" s="16"/>
-      <c r="J32" s="12"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="21"/>
       <c r="K32" s="1">
         <v>3</v>
       </c>
       <c r="L32" s="6">
         <v>45608</v>
       </c>
-      <c r="M32" s="16"/>
-      <c r="N32" s="20"/>
-      <c r="O32" s="20"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
     </row>
     <row r="33" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="16"/>
-      <c r="J33" s="12"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="21"/>
       <c r="K33" s="1">
         <v>4</v>
       </c>
       <c r="L33" s="6">
         <v>45609</v>
       </c>
-      <c r="M33" s="16"/>
-      <c r="N33" s="20"/>
-      <c r="O33" s="20"/>
+      <c r="M33" s="17"/>
+      <c r="N33" s="13"/>
+      <c r="O33" s="13"/>
     </row>
     <row r="34" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="12"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="21"/>
       <c r="K34" s="1">
         <v>5</v>
       </c>
       <c r="L34" s="6">
         <v>45610</v>
       </c>
-      <c r="M34" s="16"/>
-      <c r="N34" s="20"/>
-      <c r="O34" s="20"/>
+      <c r="M34" s="17"/>
+      <c r="N34" s="13"/>
+      <c r="O34" s="13"/>
     </row>
     <row r="35" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="17"/>
-      <c r="J35" s="12"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="21"/>
       <c r="K35" s="1">
         <v>6</v>
       </c>
       <c r="L35" s="6">
         <v>45611</v>
       </c>
-      <c r="M35" s="17"/>
-      <c r="N35" s="21"/>
-      <c r="O35" s="21"/>
+      <c r="M35" s="18"/>
+      <c r="N35" s="14"/>
+      <c r="O35" s="14"/>
     </row>
     <row r="36" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="13" t="s">
+      <c r="G36" s="21"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="J36" s="12">
+      <c r="J36" s="21">
         <v>10</v>
       </c>
       <c r="K36" s="1">
@@ -1333,87 +1333,87 @@
       <c r="L36" s="6">
         <v>45614</v>
       </c>
-      <c r="M36" s="13" t="s">
+      <c r="M36" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="N36" s="19">
+      <c r="N36" s="12">
         <v>15</v>
       </c>
-      <c r="O36" s="19" t="s">
+      <c r="O36" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="37" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G37" s="12"/>
-      <c r="H37" s="12"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="12"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="21"/>
       <c r="K37" s="1">
         <v>3</v>
       </c>
       <c r="L37" s="6">
         <v>45615</v>
       </c>
-      <c r="M37" s="14"/>
-      <c r="N37" s="20"/>
-      <c r="O37" s="20"/>
+      <c r="M37" s="20"/>
+      <c r="N37" s="13"/>
+      <c r="O37" s="13"/>
     </row>
     <row r="38" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="12"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="21"/>
       <c r="K38" s="1">
         <v>4</v>
       </c>
       <c r="L38" s="6">
         <v>45616</v>
       </c>
-      <c r="M38" s="14"/>
-      <c r="N38" s="20"/>
-      <c r="O38" s="20"/>
+      <c r="M38" s="20"/>
+      <c r="N38" s="13"/>
+      <c r="O38" s="13"/>
     </row>
     <row r="39" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G39" s="12"/>
-      <c r="H39" s="12"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="12"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="21"/>
       <c r="K39" s="1">
         <v>5</v>
       </c>
       <c r="L39" s="6">
         <v>45617</v>
       </c>
-      <c r="M39" s="14"/>
-      <c r="N39" s="20"/>
-      <c r="O39" s="20"/>
+      <c r="M39" s="20"/>
+      <c r="N39" s="13"/>
+      <c r="O39" s="13"/>
     </row>
     <row r="40" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G40" s="12"/>
-      <c r="H40" s="12"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="12"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="21"/>
       <c r="K40" s="1">
         <v>6</v>
       </c>
       <c r="L40" s="6">
         <v>45618</v>
       </c>
-      <c r="M40" s="14"/>
-      <c r="N40" s="21"/>
-      <c r="O40" s="21"/>
+      <c r="M40" s="20"/>
+      <c r="N40" s="14"/>
+      <c r="O40" s="14"/>
     </row>
     <row r="41" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G41" s="12">
+      <c r="G41" s="21">
         <v>4</v>
       </c>
-      <c r="H41" s="12" t="s">
+      <c r="H41" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I41" s="14" t="s">
+      <c r="I41" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="J41" s="12">
+      <c r="J41" s="21">
         <v>11</v>
       </c>
       <c r="K41" s="1">
@@ -1422,93 +1422,94 @@
       <c r="L41" s="6">
         <v>45621</v>
       </c>
-      <c r="M41" s="13" t="s">
+      <c r="M41" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="N41" s="19">
+      <c r="N41" s="12">
         <v>15</v>
       </c>
-      <c r="O41" s="19" t="s">
+      <c r="O41" s="12" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="42" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G42" s="12"/>
-      <c r="H42" s="12"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="12"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="21"/>
       <c r="K42" s="1">
         <v>3</v>
       </c>
       <c r="L42" s="6">
         <v>45622</v>
       </c>
-      <c r="M42" s="14"/>
-      <c r="N42" s="20"/>
-      <c r="O42" s="20"/>
+      <c r="M42" s="20"/>
+      <c r="N42" s="13"/>
+      <c r="O42" s="13"/>
     </row>
     <row r="43" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G43" s="12"/>
-      <c r="H43" s="12"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="12"/>
+      <c r="G43" s="21"/>
+      <c r="H43" s="21"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="21"/>
       <c r="K43" s="1">
         <v>4</v>
       </c>
       <c r="L43" s="6">
         <v>45623</v>
       </c>
-      <c r="M43" s="14"/>
-      <c r="N43" s="20"/>
-      <c r="O43" s="20"/>
+      <c r="M43" s="20"/>
+      <c r="N43" s="13"/>
+      <c r="O43" s="13"/>
     </row>
     <row r="44" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G44" s="12"/>
-      <c r="H44" s="12"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="12"/>
+      <c r="G44" s="21"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="20"/>
+      <c r="J44" s="21"/>
       <c r="K44" s="1">
         <v>5</v>
       </c>
       <c r="L44" s="6">
         <v>45624</v>
       </c>
-      <c r="M44" s="14"/>
-      <c r="N44" s="20"/>
-      <c r="O44" s="20"/>
+      <c r="M44" s="20"/>
+      <c r="N44" s="13"/>
+      <c r="O44" s="13"/>
     </row>
     <row r="45" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
-      <c r="I45" s="14"/>
-      <c r="J45" s="12"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="20"/>
+      <c r="J45" s="21"/>
       <c r="K45" s="1">
         <v>6</v>
       </c>
       <c r="L45" s="6">
         <v>45625</v>
       </c>
-      <c r="M45" s="14"/>
-      <c r="N45" s="21"/>
-      <c r="O45" s="21"/>
+      <c r="M45" s="20"/>
+      <c r="N45" s="14"/>
+      <c r="O45" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="O41:O45"/>
-    <mergeCell ref="O36:O40"/>
-    <mergeCell ref="O31:O35"/>
-    <mergeCell ref="N31:N35"/>
-    <mergeCell ref="M31:M35"/>
-    <mergeCell ref="M36:M40"/>
-    <mergeCell ref="N36:N40"/>
-    <mergeCell ref="M41:M45"/>
-    <mergeCell ref="N41:N45"/>
-    <mergeCell ref="N21:N25"/>
-    <mergeCell ref="M21:M25"/>
-    <mergeCell ref="O21:O25"/>
-    <mergeCell ref="M26:M30"/>
-    <mergeCell ref="N26:N30"/>
-    <mergeCell ref="O26:O30"/>
+    <mergeCell ref="J31:J35"/>
+    <mergeCell ref="G21:G30"/>
+    <mergeCell ref="H21:H30"/>
+    <mergeCell ref="I21:I25"/>
+    <mergeCell ref="I26:I30"/>
+    <mergeCell ref="G31:G40"/>
+    <mergeCell ref="H31:H40"/>
+    <mergeCell ref="I36:I40"/>
+    <mergeCell ref="J26:J30"/>
+    <mergeCell ref="J21:J25"/>
+    <mergeCell ref="I31:I35"/>
+    <mergeCell ref="G41:G45"/>
+    <mergeCell ref="H41:H45"/>
+    <mergeCell ref="I41:I45"/>
+    <mergeCell ref="J41:J45"/>
+    <mergeCell ref="J36:J40"/>
     <mergeCell ref="J16:J20"/>
     <mergeCell ref="J11:J15"/>
     <mergeCell ref="G8:O8"/>
@@ -1522,22 +1523,21 @@
     <mergeCell ref="I11:I15"/>
     <mergeCell ref="I16:I20"/>
     <mergeCell ref="O16:O20"/>
-    <mergeCell ref="G41:G45"/>
-    <mergeCell ref="H41:H45"/>
-    <mergeCell ref="I41:I45"/>
-    <mergeCell ref="J41:J45"/>
-    <mergeCell ref="J36:J40"/>
-    <mergeCell ref="J31:J35"/>
-    <mergeCell ref="G21:G30"/>
-    <mergeCell ref="H21:H30"/>
-    <mergeCell ref="I21:I25"/>
-    <mergeCell ref="I26:I30"/>
-    <mergeCell ref="G31:G40"/>
-    <mergeCell ref="H31:H40"/>
-    <mergeCell ref="I36:I40"/>
-    <mergeCell ref="J26:J30"/>
-    <mergeCell ref="J21:J25"/>
-    <mergeCell ref="I31:I35"/>
+    <mergeCell ref="N21:N25"/>
+    <mergeCell ref="M21:M25"/>
+    <mergeCell ref="O21:O25"/>
+    <mergeCell ref="M26:M30"/>
+    <mergeCell ref="N26:N30"/>
+    <mergeCell ref="O26:O30"/>
+    <mergeCell ref="O41:O45"/>
+    <mergeCell ref="O36:O40"/>
+    <mergeCell ref="O31:O35"/>
+    <mergeCell ref="N31:N35"/>
+    <mergeCell ref="M31:M35"/>
+    <mergeCell ref="M36:M40"/>
+    <mergeCell ref="N36:N40"/>
+    <mergeCell ref="M41:M45"/>
+    <mergeCell ref="N41:N45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1566,17 +1566,17 @@
   </cols>
   <sheetData>
     <row r="8" spans="7:15" ht="22.5" x14ac:dyDescent="0.6">
-      <c r="G8" s="18" t="s">
+      <c r="G8" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="22"/>
     </row>
     <row r="10" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
       <c r="G10" s="2" t="s">
@@ -1608,16 +1608,16 @@
       </c>
     </row>
     <row r="11" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G11" s="12">
+      <c r="G11" s="21">
         <v>1</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="H11" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="I11" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="J11" s="12">
+      <c r="J11" s="21">
         <v>5</v>
       </c>
       <c r="K11" s="1">
@@ -1629,84 +1629,84 @@
       <c r="M11" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="N11" s="19">
-        <v>5</v>
-      </c>
-      <c r="O11" s="15" t="s">
+      <c r="N11" s="12">
+        <v>5</v>
+      </c>
+      <c r="O11" s="16" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="12" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="12"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="21"/>
       <c r="K12" s="1">
         <v>3</v>
       </c>
       <c r="L12" s="6">
         <v>45580</v>
       </c>
-      <c r="M12" s="16" t="s">
+      <c r="M12" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="N12" s="20"/>
-      <c r="O12" s="16"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="17"/>
     </row>
     <row r="13" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="12"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="21"/>
       <c r="K13" s="1">
         <v>4</v>
       </c>
       <c r="L13" s="6">
         <v>45581</v>
       </c>
-      <c r="M13" s="16"/>
-      <c r="N13" s="20"/>
-      <c r="O13" s="16"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="17"/>
     </row>
     <row r="14" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="12"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="21"/>
       <c r="K14" s="1">
         <v>5</v>
       </c>
       <c r="L14" s="6">
         <v>45582</v>
       </c>
-      <c r="M14" s="25" t="s">
+      <c r="M14" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="N14" s="20"/>
-      <c r="O14" s="16"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="17"/>
     </row>
     <row r="15" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="12"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="21"/>
       <c r="K15" s="1">
         <v>6</v>
       </c>
       <c r="L15" s="6">
         <v>45583</v>
       </c>
-      <c r="M15" s="17"/>
-      <c r="N15" s="21"/>
-      <c r="O15" s="17"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="18"/>
     </row>
     <row r="16" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="13" t="s">
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="J16" s="12">
+      <c r="J16" s="21">
         <v>6</v>
       </c>
       <c r="K16" s="1">
@@ -1718,65 +1718,65 @@
       <c r="M16" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="N16" s="19">
-        <v>5</v>
-      </c>
-      <c r="O16" s="15" t="s">
+      <c r="N16" s="12">
+        <v>5</v>
+      </c>
+      <c r="O16" s="16" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="17" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="12"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="21"/>
       <c r="K17" s="1">
         <v>3</v>
       </c>
       <c r="L17" s="6">
         <v>45587</v>
       </c>
-      <c r="M17" s="17"/>
-      <c r="N17" s="20"/>
-      <c r="O17" s="16"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="17"/>
     </row>
     <row r="18" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="12"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="21"/>
       <c r="K18" s="1">
         <v>4</v>
       </c>
       <c r="L18" s="6">
         <v>45588</v>
       </c>
-      <c r="M18" s="15" t="s">
+      <c r="M18" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="N18" s="20"/>
-      <c r="O18" s="16"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="17"/>
     </row>
     <row r="19" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="12"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="21"/>
       <c r="K19" s="1">
         <v>5</v>
       </c>
       <c r="L19" s="6">
         <v>45589</v>
       </c>
-      <c r="M19" s="23"/>
-      <c r="N19" s="20"/>
-      <c r="O19" s="16"/>
+      <c r="M19" s="25"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="17"/>
     </row>
     <row r="20" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="12"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="21"/>
       <c r="K20" s="1">
         <v>6</v>
       </c>
@@ -1786,20 +1786,20 @@
       <c r="M20" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="N20" s="21"/>
-      <c r="O20" s="17"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="18"/>
     </row>
     <row r="21" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G21" s="12">
+      <c r="G21" s="21">
         <v>2</v>
       </c>
-      <c r="H21" s="12" t="s">
+      <c r="H21" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="I21" s="13" t="s">
+      <c r="I21" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="J21" s="12">
+      <c r="J21" s="21">
         <v>7</v>
       </c>
       <c r="K21" s="1">
@@ -1811,18 +1811,18 @@
       <c r="M21" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="N21" s="19">
-        <v>5</v>
-      </c>
-      <c r="O21" s="15" t="s">
+      <c r="N21" s="12">
+        <v>5</v>
+      </c>
+      <c r="O21" s="16" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="22" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="12"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="21"/>
       <c r="K22" s="1">
         <v>3</v>
       </c>
@@ -1832,29 +1832,29 @@
       <c r="M22" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="N22" s="20"/>
-      <c r="O22" s="16"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="17"/>
     </row>
     <row r="23" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="12"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="21"/>
       <c r="K23" s="1">
         <v>4</v>
       </c>
       <c r="L23" s="6">
         <v>45595</v>
       </c>
-      <c r="M23" s="17"/>
-      <c r="N23" s="20"/>
-      <c r="O23" s="16"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="17"/>
     </row>
     <row r="24" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="12"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="21"/>
       <c r="K24" s="1">
         <v>5</v>
       </c>
@@ -1864,31 +1864,31 @@
       <c r="M24" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="N24" s="20"/>
-      <c r="O24" s="16"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="17"/>
     </row>
     <row r="25" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="12"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="21"/>
       <c r="K25" s="1">
         <v>6</v>
       </c>
       <c r="L25" s="6">
         <v>45597</v>
       </c>
-      <c r="M25" s="17"/>
-      <c r="N25" s="21"/>
-      <c r="O25" s="17"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="14"/>
+      <c r="O25" s="18"/>
     </row>
     <row r="26" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="13" t="s">
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="J26" s="12">
+      <c r="J26" s="21">
         <v>8</v>
       </c>
       <c r="K26" s="1">
@@ -1897,51 +1897,51 @@
       <c r="L26" s="6">
         <v>45600</v>
       </c>
-      <c r="M26" s="15" t="s">
+      <c r="M26" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="N26" s="19">
-        <v>5</v>
-      </c>
-      <c r="O26" s="15" t="s">
+      <c r="N26" s="12">
+        <v>5</v>
+      </c>
+      <c r="O26" s="16" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="27" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="12"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="21"/>
       <c r="K27" s="1">
         <v>3</v>
       </c>
       <c r="L27" s="6">
         <v>45601</v>
       </c>
-      <c r="M27" s="25"/>
-      <c r="N27" s="20"/>
-      <c r="O27" s="16"/>
+      <c r="M27" s="23"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="17"/>
     </row>
     <row r="28" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="12"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="21"/>
       <c r="K28" s="1">
         <v>4</v>
       </c>
       <c r="L28" s="6">
         <v>45602</v>
       </c>
-      <c r="M28" s="23"/>
-      <c r="N28" s="20"/>
-      <c r="O28" s="16"/>
+      <c r="M28" s="25"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="17"/>
     </row>
     <row r="29" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="12"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="21"/>
       <c r="K29" s="1">
         <v>5</v>
       </c>
@@ -1951,35 +1951,35 @@
       <c r="M29" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="N29" s="20"/>
-      <c r="O29" s="16"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="17"/>
     </row>
     <row r="30" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="12"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="21"/>
       <c r="K30" s="1">
         <v>6</v>
       </c>
       <c r="L30" s="6">
         <v>45604</v>
       </c>
-      <c r="M30" s="17"/>
-      <c r="N30" s="21"/>
-      <c r="O30" s="17"/>
+      <c r="M30" s="18"/>
+      <c r="N30" s="14"/>
+      <c r="O30" s="18"/>
     </row>
     <row r="31" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G31" s="12">
+      <c r="G31" s="21">
         <v>3</v>
       </c>
-      <c r="H31" s="12" t="s">
+      <c r="H31" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="I31" s="15" t="s">
+      <c r="I31" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="J31" s="12">
+      <c r="J31" s="21">
         <v>9</v>
       </c>
       <c r="K31" s="1">
@@ -1988,83 +1988,83 @@
       <c r="L31" s="6">
         <v>45607</v>
       </c>
-      <c r="M31" s="15" t="s">
+      <c r="M31" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="N31" s="19">
-        <v>5</v>
-      </c>
-      <c r="O31" s="19" t="s">
+      <c r="N31" s="12">
+        <v>5</v>
+      </c>
+      <c r="O31" s="12" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="32" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
-      <c r="I32" s="16"/>
-      <c r="J32" s="12"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="21"/>
       <c r="K32" s="1">
         <v>3</v>
       </c>
       <c r="L32" s="6">
         <v>45608</v>
       </c>
-      <c r="M32" s="16"/>
-      <c r="N32" s="20"/>
-      <c r="O32" s="20"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
     </row>
     <row r="33" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="16"/>
-      <c r="J33" s="12"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="21"/>
       <c r="K33" s="1">
         <v>4</v>
       </c>
       <c r="L33" s="6">
         <v>45609</v>
       </c>
-      <c r="M33" s="16"/>
-      <c r="N33" s="20"/>
-      <c r="O33" s="20"/>
+      <c r="M33" s="17"/>
+      <c r="N33" s="13"/>
+      <c r="O33" s="13"/>
     </row>
     <row r="34" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="12"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="21"/>
       <c r="K34" s="1">
         <v>5</v>
       </c>
       <c r="L34" s="6">
         <v>45610</v>
       </c>
-      <c r="M34" s="16"/>
-      <c r="N34" s="20"/>
-      <c r="O34" s="20"/>
+      <c r="M34" s="17"/>
+      <c r="N34" s="13"/>
+      <c r="O34" s="13"/>
     </row>
     <row r="35" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="17"/>
-      <c r="J35" s="12"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="21"/>
       <c r="K35" s="1">
         <v>6</v>
       </c>
       <c r="L35" s="6">
         <v>45611</v>
       </c>
-      <c r="M35" s="17"/>
-      <c r="N35" s="21"/>
-      <c r="O35" s="21"/>
+      <c r="M35" s="18"/>
+      <c r="N35" s="14"/>
+      <c r="O35" s="14"/>
     </row>
     <row r="36" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="13" t="s">
+      <c r="G36" s="21"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="J36" s="12">
+      <c r="J36" s="21">
         <v>10</v>
       </c>
       <c r="K36" s="1">
@@ -2073,87 +2073,87 @@
       <c r="L36" s="6">
         <v>45614</v>
       </c>
-      <c r="M36" s="13" t="s">
+      <c r="M36" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="N36" s="19">
-        <v>5</v>
-      </c>
-      <c r="O36" s="19" t="s">
+      <c r="N36" s="12">
+        <v>5</v>
+      </c>
+      <c r="O36" s="12" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="37" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G37" s="12"/>
-      <c r="H37" s="12"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="12"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="21"/>
       <c r="K37" s="1">
         <v>3</v>
       </c>
       <c r="L37" s="6">
         <v>45615</v>
       </c>
-      <c r="M37" s="14"/>
-      <c r="N37" s="20"/>
-      <c r="O37" s="20"/>
+      <c r="M37" s="20"/>
+      <c r="N37" s="13"/>
+      <c r="O37" s="13"/>
     </row>
     <row r="38" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="12"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="21"/>
       <c r="K38" s="1">
         <v>4</v>
       </c>
       <c r="L38" s="6">
         <v>45616</v>
       </c>
-      <c r="M38" s="14"/>
-      <c r="N38" s="20"/>
-      <c r="O38" s="20"/>
+      <c r="M38" s="20"/>
+      <c r="N38" s="13"/>
+      <c r="O38" s="13"/>
     </row>
     <row r="39" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G39" s="12"/>
-      <c r="H39" s="12"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="12"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="21"/>
       <c r="K39" s="1">
         <v>5</v>
       </c>
       <c r="L39" s="6">
         <v>45617</v>
       </c>
-      <c r="M39" s="14"/>
-      <c r="N39" s="20"/>
-      <c r="O39" s="20"/>
+      <c r="M39" s="20"/>
+      <c r="N39" s="13"/>
+      <c r="O39" s="13"/>
     </row>
     <row r="40" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G40" s="12"/>
-      <c r="H40" s="12"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="12"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="21"/>
       <c r="K40" s="1">
         <v>6</v>
       </c>
       <c r="L40" s="6">
         <v>45618</v>
       </c>
-      <c r="M40" s="14"/>
-      <c r="N40" s="21"/>
-      <c r="O40" s="21"/>
+      <c r="M40" s="20"/>
+      <c r="N40" s="14"/>
+      <c r="O40" s="14"/>
     </row>
     <row r="41" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G41" s="12">
+      <c r="G41" s="21">
         <v>4</v>
       </c>
-      <c r="H41" s="12" t="s">
+      <c r="H41" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I41" s="14" t="s">
+      <c r="I41" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="J41" s="12">
+      <c r="J41" s="21">
         <v>11</v>
       </c>
       <c r="K41" s="1">
@@ -2162,78 +2162,113 @@
       <c r="L41" s="6">
         <v>45621</v>
       </c>
-      <c r="M41" s="13" t="s">
+      <c r="M41" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="N41" s="19">
-        <v>5</v>
-      </c>
-      <c r="O41" s="19" t="s">
+      <c r="N41" s="12">
+        <v>5</v>
+      </c>
+      <c r="O41" s="12" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="42" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G42" s="12"/>
-      <c r="H42" s="12"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="12"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="21"/>
       <c r="K42" s="1">
         <v>3</v>
       </c>
       <c r="L42" s="6">
         <v>45622</v>
       </c>
-      <c r="M42" s="14"/>
-      <c r="N42" s="20"/>
-      <c r="O42" s="20"/>
+      <c r="M42" s="20"/>
+      <c r="N42" s="13"/>
+      <c r="O42" s="13"/>
     </row>
     <row r="43" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G43" s="12"/>
-      <c r="H43" s="12"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="12"/>
+      <c r="G43" s="21"/>
+      <c r="H43" s="21"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="21"/>
       <c r="K43" s="1">
         <v>4</v>
       </c>
       <c r="L43" s="6">
         <v>45623</v>
       </c>
-      <c r="M43" s="14"/>
-      <c r="N43" s="20"/>
-      <c r="O43" s="20"/>
+      <c r="M43" s="20"/>
+      <c r="N43" s="13"/>
+      <c r="O43" s="13"/>
     </row>
     <row r="44" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G44" s="12"/>
-      <c r="H44" s="12"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="12"/>
+      <c r="G44" s="21"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="20"/>
+      <c r="J44" s="21"/>
       <c r="K44" s="1">
         <v>5</v>
       </c>
       <c r="L44" s="6">
         <v>45624</v>
       </c>
-      <c r="M44" s="14"/>
-      <c r="N44" s="20"/>
-      <c r="O44" s="20"/>
+      <c r="M44" s="20"/>
+      <c r="N44" s="13"/>
+      <c r="O44" s="13"/>
     </row>
     <row r="45" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
-      <c r="I45" s="14"/>
-      <c r="J45" s="12"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="20"/>
+      <c r="J45" s="21"/>
       <c r="K45" s="1">
         <v>6</v>
       </c>
       <c r="L45" s="6">
         <v>45625</v>
       </c>
-      <c r="M45" s="14"/>
-      <c r="N45" s="21"/>
-      <c r="O45" s="21"/>
+      <c r="M45" s="20"/>
+      <c r="N45" s="14"/>
+      <c r="O45" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="G8:O8"/>
+    <mergeCell ref="G11:G20"/>
+    <mergeCell ref="H11:H20"/>
+    <mergeCell ref="I11:I15"/>
+    <mergeCell ref="J11:J15"/>
+    <mergeCell ref="N11:N15"/>
+    <mergeCell ref="O11:O15"/>
+    <mergeCell ref="I16:I20"/>
+    <mergeCell ref="J16:J20"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="G21:G30"/>
+    <mergeCell ref="H21:H30"/>
+    <mergeCell ref="I21:I25"/>
+    <mergeCell ref="J21:J25"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="M26:M28"/>
+    <mergeCell ref="M29:M30"/>
+    <mergeCell ref="I26:I30"/>
+    <mergeCell ref="J26:J30"/>
+    <mergeCell ref="G31:G40"/>
+    <mergeCell ref="H31:H40"/>
+    <mergeCell ref="I31:I35"/>
+    <mergeCell ref="J31:J35"/>
+    <mergeCell ref="M31:M35"/>
+    <mergeCell ref="I36:I40"/>
+    <mergeCell ref="J36:J40"/>
+    <mergeCell ref="M36:M40"/>
+    <mergeCell ref="N36:N40"/>
+    <mergeCell ref="O36:O40"/>
+    <mergeCell ref="G41:G45"/>
+    <mergeCell ref="H41:H45"/>
+    <mergeCell ref="I41:I45"/>
+    <mergeCell ref="J41:J45"/>
+    <mergeCell ref="M41:M45"/>
     <mergeCell ref="O41:O45"/>
     <mergeCell ref="M12:M13"/>
     <mergeCell ref="M14:M15"/>
@@ -2245,43 +2280,8 @@
     <mergeCell ref="O16:O20"/>
     <mergeCell ref="N21:N25"/>
     <mergeCell ref="O21:O25"/>
-    <mergeCell ref="G41:G45"/>
-    <mergeCell ref="H41:H45"/>
-    <mergeCell ref="I41:I45"/>
-    <mergeCell ref="J41:J45"/>
-    <mergeCell ref="M41:M45"/>
     <mergeCell ref="N26:N30"/>
     <mergeCell ref="O26:O30"/>
-    <mergeCell ref="I36:I40"/>
-    <mergeCell ref="J36:J40"/>
-    <mergeCell ref="M36:M40"/>
-    <mergeCell ref="N36:N40"/>
-    <mergeCell ref="O36:O40"/>
-    <mergeCell ref="G31:G40"/>
-    <mergeCell ref="H31:H40"/>
-    <mergeCell ref="I31:I35"/>
-    <mergeCell ref="J31:J35"/>
-    <mergeCell ref="M31:M35"/>
-    <mergeCell ref="G21:G30"/>
-    <mergeCell ref="H21:H30"/>
-    <mergeCell ref="I21:I25"/>
-    <mergeCell ref="J21:J25"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="M26:M28"/>
-    <mergeCell ref="M29:M30"/>
-    <mergeCell ref="I26:I30"/>
-    <mergeCell ref="J26:J30"/>
-    <mergeCell ref="G8:O8"/>
-    <mergeCell ref="G11:G20"/>
-    <mergeCell ref="H11:H20"/>
-    <mergeCell ref="I11:I15"/>
-    <mergeCell ref="J11:J15"/>
-    <mergeCell ref="N11:N15"/>
-    <mergeCell ref="O11:O15"/>
-    <mergeCell ref="I16:I20"/>
-    <mergeCell ref="J16:J20"/>
-    <mergeCell ref="M18:M19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2339,16 +2339,16 @@
       </c>
     </row>
     <row r="4" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C4" s="12">
+      <c r="C4" s="21">
         <v>1</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="21">
         <v>5</v>
       </c>
       <c r="G4" s="1">
@@ -2360,84 +2360,84 @@
       <c r="I4" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="19">
-        <v>5</v>
-      </c>
-      <c r="K4" s="15" t="s">
+      <c r="J4" s="12">
+        <v>5</v>
+      </c>
+      <c r="K4" s="16" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="5" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="12"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="1">
         <v>3</v>
       </c>
       <c r="H5" s="10">
         <v>45580</v>
       </c>
-      <c r="I5" s="26" t="s">
+      <c r="I5" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="J5" s="20"/>
-      <c r="K5" s="16"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="17"/>
     </row>
     <row r="6" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="12"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="1">
         <v>4</v>
       </c>
       <c r="H6" s="10">
         <v>45581</v>
       </c>
-      <c r="I6" s="26"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="16"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="17"/>
     </row>
     <row r="7" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="12"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="1">
         <v>5</v>
       </c>
       <c r="H7" s="10">
         <v>45582</v>
       </c>
-      <c r="I7" s="26" t="s">
+      <c r="I7" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="20"/>
-      <c r="K7" s="16"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="17"/>
     </row>
     <row r="8" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="12"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="1">
         <v>6</v>
       </c>
       <c r="H8" s="10">
         <v>45583</v>
       </c>
-      <c r="I8" s="27"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="17"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="18"/>
     </row>
     <row r="9" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="13" t="s">
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="21">
         <v>6</v>
       </c>
       <c r="G9" s="1">
@@ -2446,68 +2446,68 @@
       <c r="H9" s="10">
         <v>45586</v>
       </c>
-      <c r="I9" s="28" t="s">
+      <c r="I9" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="J9" s="19">
-        <v>5</v>
-      </c>
-      <c r="K9" s="15" t="s">
+      <c r="J9" s="12">
+        <v>5</v>
+      </c>
+      <c r="K9" s="16" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="10" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="12"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="1">
         <v>3</v>
       </c>
       <c r="H10" s="10">
         <v>45587</v>
       </c>
-      <c r="I10" s="27"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="16"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="17"/>
     </row>
     <row r="11" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="12"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="1">
         <v>4</v>
       </c>
       <c r="H11" s="10">
         <v>45588</v>
       </c>
-      <c r="I11" s="29" t="s">
+      <c r="I11" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="J11" s="20"/>
-      <c r="K11" s="16"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="17"/>
     </row>
     <row r="12" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="12"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="21"/>
       <c r="G12" s="1">
         <v>5</v>
       </c>
       <c r="H12" s="10">
         <v>45589</v>
       </c>
-      <c r="I12" s="30"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="16"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="17"/>
     </row>
     <row r="13" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="12"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="21"/>
       <c r="G13" s="1">
         <v>6</v>
       </c>
@@ -2517,20 +2517,20 @@
       <c r="I13" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="J13" s="21"/>
-      <c r="K13" s="17"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="18"/>
     </row>
     <row r="14" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C14" s="12">
+      <c r="C14" s="21">
         <v>2</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="21">
         <v>7</v>
       </c>
       <c r="G14" s="1">
@@ -2539,83 +2539,83 @@
       <c r="H14" s="10">
         <v>45593</v>
       </c>
-      <c r="I14" s="13" t="s">
+      <c r="I14" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="J14" s="19">
+      <c r="J14" s="12">
         <v>15</v>
       </c>
-      <c r="K14" s="15" t="s">
+      <c r="K14" s="16" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="15" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="12"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="21"/>
       <c r="G15" s="1">
         <v>3</v>
       </c>
       <c r="H15" s="10">
         <v>45594</v>
       </c>
-      <c r="I15" s="14"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="16"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="17"/>
     </row>
     <row r="16" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="12"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="21"/>
       <c r="G16" s="1">
         <v>4</v>
       </c>
       <c r="H16" s="10">
         <v>45595</v>
       </c>
-      <c r="I16" s="14"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="16"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="17"/>
     </row>
     <row r="17" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="12"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="21"/>
       <c r="G17" s="1">
         <v>5</v>
       </c>
       <c r="H17" s="10">
         <v>45596</v>
       </c>
-      <c r="I17" s="14"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="16"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="17"/>
     </row>
     <row r="18" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="12"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="21"/>
       <c r="G18" s="1">
         <v>6</v>
       </c>
       <c r="H18" s="10">
         <v>45597</v>
       </c>
-      <c r="I18" s="14"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="17"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="18"/>
     </row>
     <row r="19" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="13" t="s">
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F19" s="12">
+      <c r="F19" s="21">
         <v>8</v>
       </c>
       <c r="G19" s="1">
@@ -2624,87 +2624,87 @@
       <c r="H19" s="10">
         <v>45600</v>
       </c>
-      <c r="I19" s="13" t="s">
+      <c r="I19" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="J19" s="19">
+      <c r="J19" s="12">
         <v>15</v>
       </c>
-      <c r="K19" s="15" t="s">
+      <c r="K19" s="16" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="20" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="12"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="21"/>
       <c r="G20" s="1">
         <v>3</v>
       </c>
       <c r="H20" s="10">
         <v>45601</v>
       </c>
-      <c r="I20" s="14"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="16"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="17"/>
     </row>
     <row r="21" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="12"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="21"/>
       <c r="G21" s="1">
         <v>4</v>
       </c>
       <c r="H21" s="10">
         <v>45602</v>
       </c>
-      <c r="I21" s="14"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="16"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="17"/>
     </row>
     <row r="22" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="12"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="21"/>
       <c r="G22" s="1">
         <v>5</v>
       </c>
       <c r="H22" s="10">
         <v>45603</v>
       </c>
-      <c r="I22" s="14"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="16"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="17"/>
     </row>
     <row r="23" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="12"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="21"/>
       <c r="G23" s="1">
         <v>6</v>
       </c>
       <c r="H23" s="10">
         <v>45604</v>
       </c>
-      <c r="I23" s="14"/>
-      <c r="J23" s="21"/>
-      <c r="K23" s="17"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="18"/>
     </row>
     <row r="24" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C24" s="12">
+      <c r="C24" s="21">
         <v>3</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="E24" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F24" s="21">
         <v>9</v>
       </c>
       <c r="G24" s="1">
@@ -2713,83 +2713,83 @@
       <c r="H24" s="10">
         <v>45607</v>
       </c>
-      <c r="I24" s="13" t="s">
+      <c r="I24" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="J24" s="19">
+      <c r="J24" s="12">
         <v>15</v>
       </c>
-      <c r="K24" s="19" t="s">
+      <c r="K24" s="12" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="25" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="12"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="21"/>
       <c r="G25" s="1">
         <v>3</v>
       </c>
       <c r="H25" s="10">
         <v>45608</v>
       </c>
-      <c r="I25" s="14"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
     </row>
     <row r="26" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="12"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="21"/>
       <c r="G26" s="1">
         <v>4</v>
       </c>
       <c r="H26" s="10">
         <v>45609</v>
       </c>
-      <c r="I26" s="14"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
     </row>
     <row r="27" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="12"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="21"/>
       <c r="G27" s="1">
         <v>5</v>
       </c>
       <c r="H27" s="10">
         <v>45610</v>
       </c>
-      <c r="I27" s="14"/>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
     </row>
     <row r="28" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="12"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="21"/>
       <c r="G28" s="1">
         <v>6</v>
       </c>
       <c r="H28" s="10">
         <v>45611</v>
       </c>
-      <c r="I28" s="14"/>
-      <c r="J28" s="21"/>
-      <c r="K28" s="21"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
     </row>
     <row r="29" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="14" t="s">
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="F29" s="12">
+      <c r="F29" s="21">
         <v>10</v>
       </c>
       <c r="G29" s="1">
@@ -2798,87 +2798,87 @@
       <c r="H29" s="10">
         <v>45614</v>
       </c>
-      <c r="I29" s="14" t="s">
+      <c r="I29" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="J29" s="19">
+      <c r="J29" s="12">
         <v>15</v>
       </c>
-      <c r="K29" s="19" t="s">
+      <c r="K29" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="30" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="12"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="21"/>
       <c r="G30" s="1">
         <v>3</v>
       </c>
       <c r="H30" s="10">
         <v>45615</v>
       </c>
-      <c r="I30" s="14"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
     </row>
     <row r="31" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="12"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="21"/>
       <c r="G31" s="1">
         <v>4</v>
       </c>
       <c r="H31" s="10">
         <v>45616</v>
       </c>
-      <c r="I31" s="14"/>
-      <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
     </row>
     <row r="32" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="12"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="1">
         <v>5</v>
       </c>
       <c r="H32" s="10">
         <v>45617</v>
       </c>
-      <c r="I32" s="14"/>
-      <c r="J32" s="20"/>
-      <c r="K32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
     </row>
     <row r="33" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="12"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="21"/>
       <c r="G33" s="1">
         <v>6</v>
       </c>
       <c r="H33" s="10">
         <v>45618</v>
       </c>
-      <c r="I33" s="14"/>
-      <c r="J33" s="21"/>
-      <c r="K33" s="21"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="14"/>
     </row>
     <row r="34" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C34" s="12">
+      <c r="C34" s="21">
         <v>4</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D34" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="E34" s="14" t="s">
+      <c r="E34" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="F34" s="12">
+      <c r="F34" s="21">
         <v>11</v>
       </c>
       <c r="G34" s="1">
@@ -2887,102 +2887,83 @@
       <c r="H34" s="10">
         <v>45621</v>
       </c>
-      <c r="I34" s="13" t="s">
+      <c r="I34" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="J34" s="19">
+      <c r="J34" s="12">
         <v>15</v>
       </c>
-      <c r="K34" s="19" t="s">
+      <c r="K34" s="12" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="35" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="12"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="21"/>
       <c r="G35" s="1">
         <v>3</v>
       </c>
       <c r="H35" s="10">
         <v>45622</v>
       </c>
-      <c r="I35" s="14"/>
-      <c r="J35" s="20"/>
-      <c r="K35" s="20"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
     </row>
     <row r="36" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="12"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="21"/>
       <c r="G36" s="1">
         <v>4</v>
       </c>
       <c r="H36" s="10">
         <v>45623</v>
       </c>
-      <c r="I36" s="14"/>
-      <c r="J36" s="20"/>
-      <c r="K36" s="20"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
     </row>
     <row r="37" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="12"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="21"/>
       <c r="G37" s="1">
         <v>5</v>
       </c>
       <c r="H37" s="10">
         <v>45624</v>
       </c>
-      <c r="I37" s="14"/>
-      <c r="J37" s="20"/>
-      <c r="K37" s="20"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
     </row>
     <row r="38" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="12"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="21"/>
       <c r="G38" s="1">
         <v>6</v>
       </c>
       <c r="H38" s="10">
         <v>45625</v>
       </c>
-      <c r="I38" s="14"/>
-      <c r="J38" s="21"/>
-      <c r="K38" s="21"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="K34:K38"/>
-    <mergeCell ref="C34:C38"/>
-    <mergeCell ref="D34:D38"/>
-    <mergeCell ref="E34:E38"/>
-    <mergeCell ref="F34:F38"/>
-    <mergeCell ref="I34:I38"/>
-    <mergeCell ref="J34:J38"/>
-    <mergeCell ref="K24:K28"/>
-    <mergeCell ref="E29:E33"/>
-    <mergeCell ref="F29:F33"/>
-    <mergeCell ref="I29:I33"/>
-    <mergeCell ref="J29:J33"/>
-    <mergeCell ref="K29:K33"/>
-    <mergeCell ref="J24:J28"/>
-    <mergeCell ref="C24:C33"/>
-    <mergeCell ref="D24:D33"/>
-    <mergeCell ref="E24:E28"/>
-    <mergeCell ref="F24:F28"/>
-    <mergeCell ref="I24:I28"/>
-    <mergeCell ref="E19:E23"/>
-    <mergeCell ref="F19:F23"/>
-    <mergeCell ref="I19:I23"/>
-    <mergeCell ref="J19:J23"/>
-    <mergeCell ref="K19:K23"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="E9:E13"/>
+    <mergeCell ref="F9:F13"/>
+    <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J13"/>
     <mergeCell ref="K9:K13"/>
     <mergeCell ref="I11:I12"/>
@@ -2999,11 +2980,30 @@
     <mergeCell ref="J4:J8"/>
     <mergeCell ref="K4:K8"/>
     <mergeCell ref="K14:K18"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="E9:E13"/>
-    <mergeCell ref="F9:F13"/>
-    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="E19:E23"/>
+    <mergeCell ref="F19:F23"/>
+    <mergeCell ref="I19:I23"/>
+    <mergeCell ref="J19:J23"/>
+    <mergeCell ref="K19:K23"/>
+    <mergeCell ref="C24:C33"/>
+    <mergeCell ref="D24:D33"/>
+    <mergeCell ref="E24:E28"/>
+    <mergeCell ref="F24:F28"/>
+    <mergeCell ref="I24:I28"/>
+    <mergeCell ref="K24:K28"/>
+    <mergeCell ref="E29:E33"/>
+    <mergeCell ref="F29:F33"/>
+    <mergeCell ref="I29:I33"/>
+    <mergeCell ref="J29:J33"/>
+    <mergeCell ref="K29:K33"/>
+    <mergeCell ref="J24:J28"/>
+    <mergeCell ref="K34:K38"/>
+    <mergeCell ref="C34:C38"/>
+    <mergeCell ref="D34:D38"/>
+    <mergeCell ref="E34:E38"/>
+    <mergeCell ref="F34:F38"/>
+    <mergeCell ref="I34:I38"/>
+    <mergeCell ref="J34:J38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3060,16 +3060,16 @@
       </c>
     </row>
     <row r="6" spans="3:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="C6" s="12">
+      <c r="C6" s="21">
         <v>1</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="21">
         <v>5</v>
       </c>
       <c r="G6" s="10">
@@ -3081,18 +3081,18 @@
       <c r="I6" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="J6" s="19">
+      <c r="J6" s="12">
         <v>15</v>
       </c>
-      <c r="K6" s="15" t="s">
+      <c r="K6" s="16" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="7" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="12"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="10">
         <v>45580</v>
       </c>
@@ -3102,14 +3102,14 @@
       <c r="I7" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="J7" s="20"/>
-      <c r="K7" s="16"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="17"/>
     </row>
     <row r="8" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="12"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="10">
         <v>45581</v>
       </c>
@@ -3119,14 +3119,14 @@
       <c r="I8" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="J8" s="20"/>
-      <c r="K8" s="16"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="17"/>
     </row>
     <row r="9" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="12"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="10">
         <v>45582</v>
       </c>
@@ -3136,16 +3136,16 @@
       <c r="I9" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="J9" s="20"/>
-      <c r="K9" s="16"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="17"/>
     </row>
     <row r="10" spans="3:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="13" t="s">
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="21">
         <v>6</v>
       </c>
       <c r="G10" s="10">
@@ -3157,18 +3157,18 @@
       <c r="I10" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="J10" s="19">
+      <c r="J10" s="12">
         <v>15</v>
       </c>
-      <c r="K10" s="15" t="s">
+      <c r="K10" s="16" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="11" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="12"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="10">
         <v>45587</v>
       </c>
@@ -3178,14 +3178,14 @@
       <c r="I11" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="J11" s="20"/>
-      <c r="K11" s="16"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="17"/>
     </row>
     <row r="12" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="12"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="21"/>
       <c r="G12" s="10">
         <v>45588</v>
       </c>
@@ -3195,14 +3195,14 @@
       <c r="I12" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="J12" s="20"/>
-      <c r="K12" s="16"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="17"/>
     </row>
     <row r="13" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="12"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="21"/>
       <c r="G13" s="10">
         <v>45589</v>
       </c>
@@ -3212,20 +3212,20 @@
       <c r="I13" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="J13" s="20"/>
-      <c r="K13" s="16"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="17"/>
     </row>
     <row r="14" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C14" s="12">
+      <c r="C14" s="21">
         <v>2</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="21">
         <v>7</v>
       </c>
       <c r="G14" s="10">
@@ -3234,83 +3234,83 @@
       <c r="H14" s="1">
         <v>2</v>
       </c>
-      <c r="I14" s="13" t="s">
+      <c r="I14" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="J14" s="19">
+      <c r="J14" s="12">
         <v>15</v>
       </c>
-      <c r="K14" s="15" t="s">
+      <c r="K14" s="16" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="15" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="12"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="21"/>
       <c r="G15" s="10">
         <v>45594</v>
       </c>
       <c r="H15" s="1">
         <v>3</v>
       </c>
-      <c r="I15" s="14"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="16"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="17"/>
     </row>
     <row r="16" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="12"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="21"/>
       <c r="G16" s="10">
         <v>45595</v>
       </c>
       <c r="H16" s="1">
         <v>4</v>
       </c>
-      <c r="I16" s="14"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="16"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="17"/>
     </row>
     <row r="17" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="12"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="21"/>
       <c r="G17" s="10">
         <v>45596</v>
       </c>
       <c r="H17" s="1">
         <v>5</v>
       </c>
-      <c r="I17" s="14"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="16"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="17"/>
     </row>
     <row r="18" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="12"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="21"/>
       <c r="G18" s="10">
         <v>45597</v>
       </c>
       <c r="H18" s="1">
         <v>6</v>
       </c>
-      <c r="I18" s="14"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="17"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="18"/>
     </row>
     <row r="19" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="13" t="s">
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F19" s="12">
+      <c r="F19" s="21">
         <v>8</v>
       </c>
       <c r="G19" s="10">
@@ -3319,87 +3319,87 @@
       <c r="H19" s="1">
         <v>2</v>
       </c>
-      <c r="I19" s="13" t="s">
+      <c r="I19" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="J19" s="19">
+      <c r="J19" s="12">
         <v>15</v>
       </c>
-      <c r="K19" s="15" t="s">
+      <c r="K19" s="16" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="20" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="12"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="21"/>
       <c r="G20" s="10">
         <v>45601</v>
       </c>
       <c r="H20" s="1">
         <v>3</v>
       </c>
-      <c r="I20" s="14"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="16"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="17"/>
     </row>
     <row r="21" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="12"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="21"/>
       <c r="G21" s="10">
         <v>45602</v>
       </c>
       <c r="H21" s="1">
         <v>4</v>
       </c>
-      <c r="I21" s="14"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="16"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="17"/>
     </row>
     <row r="22" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="12"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="21"/>
       <c r="G22" s="10">
         <v>45603</v>
       </c>
       <c r="H22" s="1">
         <v>5</v>
       </c>
-      <c r="I22" s="14"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="16"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="17"/>
     </row>
     <row r="23" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="12"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="21"/>
       <c r="G23" s="10">
         <v>45604</v>
       </c>
       <c r="H23" s="1">
         <v>6</v>
       </c>
-      <c r="I23" s="14"/>
-      <c r="J23" s="21"/>
-      <c r="K23" s="17"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="18"/>
     </row>
     <row r="24" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C24" s="12">
+      <c r="C24" s="21">
         <v>3</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="E24" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F24" s="21">
         <v>9</v>
       </c>
       <c r="G24" s="10">
@@ -3408,83 +3408,83 @@
       <c r="H24" s="1">
         <v>2</v>
       </c>
-      <c r="I24" s="13" t="s">
+      <c r="I24" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="J24" s="19">
+      <c r="J24" s="12">
         <v>15</v>
       </c>
-      <c r="K24" s="19" t="s">
+      <c r="K24" s="12" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="25" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="12"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="21"/>
       <c r="G25" s="10">
         <v>45608</v>
       </c>
       <c r="H25" s="1">
         <v>3</v>
       </c>
-      <c r="I25" s="14"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
     </row>
     <row r="26" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="12"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="21"/>
       <c r="G26" s="10">
         <v>45609</v>
       </c>
       <c r="H26" s="1">
         <v>4</v>
       </c>
-      <c r="I26" s="14"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
     </row>
     <row r="27" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="12"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="21"/>
       <c r="G27" s="10">
         <v>45610</v>
       </c>
       <c r="H27" s="1">
         <v>5</v>
       </c>
-      <c r="I27" s="14"/>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
     </row>
     <row r="28" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="12"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="21"/>
       <c r="G28" s="10">
         <v>45611</v>
       </c>
       <c r="H28" s="1">
         <v>6</v>
       </c>
-      <c r="I28" s="14"/>
-      <c r="J28" s="21"/>
-      <c r="K28" s="21"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
     </row>
     <row r="29" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="14" t="s">
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="F29" s="12">
+      <c r="F29" s="21">
         <v>10</v>
       </c>
       <c r="G29" s="10">
@@ -3493,87 +3493,87 @@
       <c r="H29" s="1">
         <v>2</v>
       </c>
-      <c r="I29" s="14" t="s">
+      <c r="I29" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="J29" s="19">
+      <c r="J29" s="12">
         <v>15</v>
       </c>
-      <c r="K29" s="19" t="s">
+      <c r="K29" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="30" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="12"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="21"/>
       <c r="G30" s="10">
         <v>45615</v>
       </c>
       <c r="H30" s="1">
         <v>3</v>
       </c>
-      <c r="I30" s="14"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
     </row>
     <row r="31" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="12"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="21"/>
       <c r="G31" s="10">
         <v>45616</v>
       </c>
       <c r="H31" s="1">
         <v>4</v>
       </c>
-      <c r="I31" s="14"/>
-      <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
     </row>
     <row r="32" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="12"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="10">
         <v>45617</v>
       </c>
       <c r="H32" s="1">
         <v>5</v>
       </c>
-      <c r="I32" s="14"/>
-      <c r="J32" s="20"/>
-      <c r="K32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
     </row>
     <row r="33" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="12"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="21"/>
       <c r="G33" s="10">
         <v>45618</v>
       </c>
       <c r="H33" s="1">
         <v>6</v>
       </c>
-      <c r="I33" s="14"/>
-      <c r="J33" s="21"/>
-      <c r="K33" s="21"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="14"/>
     </row>
     <row r="34" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C34" s="12">
+      <c r="C34" s="21">
         <v>4</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D34" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="E34" s="14" t="s">
+      <c r="E34" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="F34" s="12">
+      <c r="F34" s="21">
         <v>11</v>
       </c>
       <c r="G34" s="10">
@@ -3582,78 +3582,112 @@
       <c r="H34" s="1">
         <v>2</v>
       </c>
-      <c r="I34" s="13" t="s">
+      <c r="I34" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="J34" s="19">
+      <c r="J34" s="12">
         <v>15</v>
       </c>
-      <c r="K34" s="19" t="s">
+      <c r="K34" s="12" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="35" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="12"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="21"/>
       <c r="G35" s="10">
         <v>45622</v>
       </c>
       <c r="H35" s="1">
         <v>3</v>
       </c>
-      <c r="I35" s="14"/>
-      <c r="J35" s="20"/>
-      <c r="K35" s="20"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
     </row>
     <row r="36" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="12"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="21"/>
       <c r="G36" s="10">
         <v>45623</v>
       </c>
       <c r="H36" s="1">
         <v>4</v>
       </c>
-      <c r="I36" s="14"/>
-      <c r="J36" s="20"/>
-      <c r="K36" s="20"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
     </row>
     <row r="37" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="12"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="21"/>
       <c r="G37" s="10">
         <v>45624</v>
       </c>
       <c r="H37" s="1">
         <v>5</v>
       </c>
-      <c r="I37" s="14"/>
-      <c r="J37" s="20"/>
-      <c r="K37" s="20"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
     </row>
     <row r="38" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="12"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="21"/>
       <c r="G38" s="10">
         <v>45625</v>
       </c>
       <c r="H38" s="1">
         <v>6</v>
       </c>
-      <c r="I38" s="14"/>
-      <c r="J38" s="21"/>
-      <c r="K38" s="21"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="K6:K9"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="J10:J13"/>
+    <mergeCell ref="K10:K13"/>
+    <mergeCell ref="C6:C13"/>
+    <mergeCell ref="D6:D13"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="F6:F9"/>
+    <mergeCell ref="J6:J9"/>
+    <mergeCell ref="C14:C23"/>
+    <mergeCell ref="D14:D23"/>
+    <mergeCell ref="E14:E18"/>
+    <mergeCell ref="F14:F18"/>
+    <mergeCell ref="I14:I18"/>
+    <mergeCell ref="K14:K18"/>
+    <mergeCell ref="E19:E23"/>
+    <mergeCell ref="F19:F23"/>
+    <mergeCell ref="I19:I23"/>
+    <mergeCell ref="J19:J23"/>
+    <mergeCell ref="K19:K23"/>
+    <mergeCell ref="J14:J18"/>
+    <mergeCell ref="C24:C33"/>
+    <mergeCell ref="D24:D33"/>
+    <mergeCell ref="E24:E28"/>
+    <mergeCell ref="F24:F28"/>
+    <mergeCell ref="I24:I28"/>
+    <mergeCell ref="K24:K28"/>
+    <mergeCell ref="E29:E33"/>
+    <mergeCell ref="F29:F33"/>
+    <mergeCell ref="I29:I33"/>
+    <mergeCell ref="J29:J33"/>
+    <mergeCell ref="K29:K33"/>
+    <mergeCell ref="J24:J28"/>
     <mergeCell ref="K34:K38"/>
     <mergeCell ref="C34:C38"/>
     <mergeCell ref="D34:D38"/>
@@ -3661,40 +3695,6 @@
     <mergeCell ref="F34:F38"/>
     <mergeCell ref="I34:I38"/>
     <mergeCell ref="J34:J38"/>
-    <mergeCell ref="K24:K28"/>
-    <mergeCell ref="E29:E33"/>
-    <mergeCell ref="F29:F33"/>
-    <mergeCell ref="I29:I33"/>
-    <mergeCell ref="J29:J33"/>
-    <mergeCell ref="K29:K33"/>
-    <mergeCell ref="J24:J28"/>
-    <mergeCell ref="C24:C33"/>
-    <mergeCell ref="D24:D33"/>
-    <mergeCell ref="E24:E28"/>
-    <mergeCell ref="F24:F28"/>
-    <mergeCell ref="I24:I28"/>
-    <mergeCell ref="K14:K18"/>
-    <mergeCell ref="E19:E23"/>
-    <mergeCell ref="F19:F23"/>
-    <mergeCell ref="I19:I23"/>
-    <mergeCell ref="J19:J23"/>
-    <mergeCell ref="K19:K23"/>
-    <mergeCell ref="J14:J18"/>
-    <mergeCell ref="C14:C23"/>
-    <mergeCell ref="D14:D23"/>
-    <mergeCell ref="E14:E18"/>
-    <mergeCell ref="F14:F18"/>
-    <mergeCell ref="I14:I18"/>
-    <mergeCell ref="C6:C13"/>
-    <mergeCell ref="D6:D13"/>
-    <mergeCell ref="E6:E9"/>
-    <mergeCell ref="F6:F9"/>
-    <mergeCell ref="J6:J9"/>
-    <mergeCell ref="K6:K9"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="F10:F13"/>
-    <mergeCell ref="J10:J13"/>
-    <mergeCell ref="K10:K13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Tong hop sprint tong gd 4 sprint 2
</commit_message>
<xml_diff>
--- a/PTUD/CDUD - 2/files/Nhom2 - CDUD2 - Sprints.xlsx
+++ b/PTUD/CDUD - 2/files/Nhom2 - CDUD2 - Sprints.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CDUD2\Chuyen-De-Phat-Trien-Ung-Dung---TDC---2024\PTUD\CDUD - 2\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\NhatTaiC\Chuyen-De-Phat-Trien-Ung-Dung---TDC---2024\PTUD\CDUD - 2\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE3A687-3C5E-40B8-AC8C-D67E19B356F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="21804" windowHeight="12984" activeTab="2"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint Tổng" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="94">
   <si>
     <t>STT</t>
   </si>
@@ -138,9 +139,6 @@
     <t>hoàn thành form loại hàng</t>
   </si>
   <si>
-    <t>Thiết kế report Hóa đơn</t>
-  </si>
-  <si>
     <t>1. Code 9 forms tiếp theo.
 2. Sửa UI và Viết Testcase cho 9 forms tiếp theo.
 3. Thêm dữ liệu mẫu cho DB.</t>
@@ -149,11 +147,6 @@
     <t>1. Chi tiết phiếu nhập, ca làm, lịch làm (Văn Toàn)
 2. Bảng lương, chi tiết bảng lương, chi nhánh (Quốc Lượng)
 3. Khuyến mãi, hóa đơn, chi tiết hóa đơn (Nhật Tài)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Hoàn thành 6 forms tra cứu thông tin tiếp theo.
-2. Hoàn thành sửa UI và Viết Testcase cho 6 forms tiếp theo.
-</t>
   </si>
   <si>
     <t>Thêm dữ liệu mẫu cho DB form tài khoản, nhà cung cấp, loại hàng</t>
@@ -177,44 +170,8 @@
 4. Hoàn thành dữ liệu mẫu cho UD QLST</t>
   </si>
   <si>
-    <t>1. Hoàn thành 9 forms tra cứu thông tin.
-2. Hoàn thành sửa UI và Viết Testcase cho 9 forms.
-3. Hoàn thành design report Hóa đơn, Thống kê doanh thu theo tháng/năm, Danh sách sản phẩm.</t>
-  </si>
-  <si>
-    <t>Code form tra cứu tài khoản, nhà cung cấp, loại hàng</t>
-  </si>
-  <si>
-    <t>Sửa UI và viết Testcase cho form tra cứu tài khoản, nhà cung cấp, loại hàng</t>
-  </si>
-  <si>
-    <t>1. Tra cứu khuyến mãi, hóa đơn (Nhật Tài)</t>
-  </si>
-  <si>
-    <t>Code 2 form tra cứu khuyến mãi, hóa đơn</t>
-  </si>
-  <si>
-    <t>Sửa UI và viết Testcase cho 2 form khuyến mãi, hóa đơn</t>
-  </si>
-  <si>
     <t>1. Hoàn thành các Task, kiểm tra Dữ liệu DB.
 2. Hoàn thành tài liệu SRS (cập nhật lại)</t>
-  </si>
-  <si>
-    <t>1. Hoàn thành form bán hàng
-2. Viết testcase &amp; sửa UI cho form bán hàng
-3. Hoàn thành kiểm tra kết nối DB, đóng gói project.</t>
-  </si>
-  <si>
-    <t>1,2. Nhật Tài</t>
-  </si>
-  <si>
-    <t>1. Kiểm tra dữ liệu DB.
-2. Kiểm tra tài liệu SRS (cập nhật lại).</t>
-  </si>
-  <si>
-    <t>1. Tổng hợp code QLST.
-2. Kiểm tra kết nối DB, đóng gói project.</t>
   </si>
   <si>
     <t>1. Đăng nhập, màn hình chính, tài khoản, loại nhân viên, nhân viên (Nhật Tài)</t>
@@ -225,10 +182,6 @@
 3. Phiếu nhập, khách hàng, nhà cung cấp (Văn Toàn)</t>
   </si>
   <si>
-    <t>1.Tra cứu tài khoản, loại nhân viên, nhân viên. (Nhật Tài)
-2. Thiết kế report Hóa đơn. (Nhật Tài)</t>
-  </si>
-  <si>
     <t>Code 3 form nhà cung cấp, phiếu nhập, khách hàng</t>
   </si>
   <si>
@@ -243,46 +196,11 @@
   </si>
   <si>
     <t>Cập nhật và chỉnh sửa SRS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.Tra cứu nhân viên. (Nhật Tài)
-2. Tra cứu  khách hàng (Văn Toàn)
-3. Tra cứu sản phẩm (Quốc Lượng)
-4. Code và test Form Bán hàng(Quốc Lượng, Văn toàn)
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Hoàn thành code 3 chức năng tra cứu thông tin.
-2. Hoàn thành Sửa UI và Viết Testcase cho 4 forms.
-3. Hoàn  thành code form bán hàng.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Code 3 chức năng tra cứu thông tin.
-2. Sửa UI và Viết Testcase cho 4 forms.
-3. Code form bán hàng.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Tra cứu lịch làm (Văn Toàn)
-2. Tra cứu bảng lương (Quốc Lượng)
-3. Thiết kế report Hóa đơn và tra cứu hóa đơn (Nhật Tài)
-</t>
   </si>
   <si>
     <t xml:space="preserve">1. Hoàn thành 3 chức năng tra cứu thông tin tiếp theo.
 2. Hoàn thành sửa UI và Viết Testcase cho 3 chức năng tiếp theo.
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Code 3 chức năng tra cứu thông tin tiếp theo.
-</t>
-  </si>
-  <si>
-    <t>1. Kiểm tra các Task, dữ liệu db.
-2. Kiểm tra tài liệu SRS (cập nhật lại).
-1. Viết testcase &amp; sửa UI cho form bán hàng.
-2. Kiểm tra kết nối DB, đóng gói project.</t>
   </si>
   <si>
     <t>1. Báo cáo kt môn.</t>
@@ -294,11 +212,6 @@
 3. Tổng hợp testcase trong tài liệu SRS (Nhật Tài)</t>
   </si>
   <si>
-    <t>1. Report Thống kê doanh thu theo tháng/năm, Tạo database khi chạy phần mềm  (Quốc Lượng)
-2. Report lợi nhuận theo tháng.
-3. Tổng hợp testcase trong tài liệu SRS.</t>
-  </si>
-  <si>
     <t>1. Hoàn thành report Thống kê doanh thu theo tháng/năm, Tạo database khi chạy phần mềm 
 2. Hoàn thành report lợi nhuận theo tháng
 3. Tổng hợp testcase trong tài liệu SRS</t>
@@ -384,12 +297,77 @@
   </si>
   <si>
     <t>code hoàn chỉnh report lợi nhuận</t>
+  </si>
+  <si>
+    <t>1. Kiểm tra các Task, kiểm tra Dữ liệu DB.
+2. Kiểm tra tài liệu SRS (cập nhật lại).</t>
+  </si>
+  <si>
+    <t>1. Report Thống kê doanh thu theo tháng/năm, Tạo database khi chạy phần mềm  (Quốc Lượng)
+2. Report lợi nhuận theo tháng. (Văn Toàn)
+3. Tổng hợp testcase trong tài liệu SRS. (Nhật Tài)</t>
+  </si>
+  <si>
+    <t>1. Hoàn thành report Thống kê doanh thu theo tháng/năm, Tạo database khi chạy phần mềm 
+2. Hoàn thành report lợi nhuận theo tháng. (Văn Toàn)
+3. Tổng hợp testcase trong tài liệu SRS. (Nhật Tài)</t>
+  </si>
+  <si>
+    <t>1. Code 3 chức năng tra cứu thông tin.
+2. Sửa UI và Viết Testcase cho 4 forms.
+3. Code form bán hàng.</t>
+  </si>
+  <si>
+    <t>1. Code 3 chức năng tra cứu thông tin tiếp theo.</t>
+  </si>
+  <si>
+    <t>1. Hoàn thành 3 chức năng tra cứu thông tin tiếp theo.</t>
+  </si>
+  <si>
+    <t>1. Hoàn thành code 3 chức năng tra cứu thông tin.
+2. Hoàn thành Sửa UI và Viết Testcase cho 4 forms.
+3. Hoàn  thành code form bán hàng.</t>
+  </si>
+  <si>
+    <t>1.Tra cứu nhân viên. (Nhật Tài)
+2. Tra cứu  khách hàng (Văn Toàn)
+3. Tra cứu sản phẩm (Quốc Lượng)
+4. Code và test Form Bán hàng(Quốc Lượng, Văn toàn)</t>
+  </si>
+  <si>
+    <t>1. Tra cứu lịch làm (Văn Toàn)
+2. Tra cứu bảng lương (Quốc Lượng)
+3. Thiết kế report Hóa đơn và tra cứu hóa đơn (Nhật Tài)</t>
+  </si>
+  <si>
+    <t>1.Tra cứu nhân viên. (Nhật Tài)</t>
+  </si>
+  <si>
+    <t>Code form tra cứu nhân viên</t>
+  </si>
+  <si>
+    <t>Sửa UI và viết Testcase cho form nhân viên</t>
+  </si>
+  <si>
+    <t>1. Thiết kế report Hóa đơn và tra cứu hóa đơn (Nhật Tài)</t>
+  </si>
+  <si>
+    <t>Code frm tra cứu hóa đơn và thiết kế report</t>
+  </si>
+  <si>
+    <t>Sửa UI và viết Testcase cho hóa đơn</t>
+  </si>
+  <si>
+    <t>1. Tổng hợp testcase trong tài liệu SRS (Nhật Tài)</t>
+  </si>
+  <si>
+    <t>Nhóm 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
@@ -565,14 +543,14 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -582,15 +560,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -605,19 +574,31 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -629,13 +610,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -916,40 +894,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="G8:O45"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36:I40"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="7" max="7" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="35.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="89" customWidth="1"/>
+    <col min="7" max="7" width="5.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="52.53125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.06640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.53125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="85.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="7:15" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="G8" s="22" t="s">
+    <row r="8" spans="7:15" ht="22.5" x14ac:dyDescent="0.6">
+      <c r="G8" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22"/>
-      <c r="O8" s="22"/>
-    </row>
-    <row r="10" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
+    </row>
+    <row r="10" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
       <c r="G10" s="2" t="s">
         <v>0</v>
       </c>
@@ -978,17 +956,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G11" s="21">
+    <row r="11" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G11" s="13">
         <v>1</v>
       </c>
-      <c r="H11" s="21" t="s">
+      <c r="H11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="I11" s="19" t="s">
+      <c r="I11" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="J11" s="21">
+      <c r="J11" s="13">
         <v>5</v>
       </c>
       <c r="K11" s="1">
@@ -1000,18 +978,18 @@
       <c r="M11" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="N11" s="13">
+      <c r="N11" s="23">
         <v>15</v>
       </c>
-      <c r="O11" s="23" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="21"/>
+      <c r="O11" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="13"/>
       <c r="K12" s="1">
         <v>3</v>
       </c>
@@ -1019,14 +997,14 @@
         <v>45580</v>
       </c>
       <c r="M12" s="17"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="24"/>
-    </row>
-    <row r="13" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="21"/>
+      <c r="N12" s="24"/>
+      <c r="O12" s="21"/>
+    </row>
+    <row r="13" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="13"/>
       <c r="K13" s="1">
         <v>4</v>
       </c>
@@ -1034,14 +1012,14 @@
         <v>45581</v>
       </c>
       <c r="M13" s="17"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="24"/>
-    </row>
-    <row r="14" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="21"/>
+      <c r="N13" s="24"/>
+      <c r="O13" s="21"/>
+    </row>
+    <row r="14" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="13"/>
       <c r="K14" s="1">
         <v>5</v>
       </c>
@@ -1049,14 +1027,14 @@
         <v>45582</v>
       </c>
       <c r="M14" s="17"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="24"/>
-    </row>
-    <row r="15" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="21"/>
+      <c r="N14" s="24"/>
+      <c r="O14" s="21"/>
+    </row>
+    <row r="15" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="13"/>
       <c r="K15" s="1">
         <v>6</v>
       </c>
@@ -1064,16 +1042,16 @@
         <v>45583</v>
       </c>
       <c r="M15" s="18"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="25"/>
-    </row>
-    <row r="16" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="19" t="s">
+      <c r="N15" s="25"/>
+      <c r="O15" s="22"/>
+    </row>
+    <row r="16" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="J16" s="21">
+      <c r="J16" s="13">
         <v>6</v>
       </c>
       <c r="K16" s="1">
@@ -1082,87 +1060,87 @@
       <c r="L16" s="6">
         <v>45586</v>
       </c>
-      <c r="M16" s="19" t="s">
+      <c r="M16" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="N16" s="23">
+        <v>15</v>
+      </c>
+      <c r="O16" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="N16" s="13">
-        <v>15</v>
-      </c>
-      <c r="O16" s="16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="21"/>
+    </row>
+    <row r="17" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="13"/>
       <c r="K17" s="1">
         <v>3</v>
       </c>
       <c r="L17" s="6">
         <v>45587</v>
       </c>
-      <c r="M17" s="20"/>
-      <c r="N17" s="14"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="24"/>
       <c r="O17" s="17"/>
     </row>
-    <row r="18" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="21"/>
+    <row r="18" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="13"/>
       <c r="K18" s="1">
         <v>4</v>
       </c>
       <c r="L18" s="6">
         <v>45588</v>
       </c>
-      <c r="M18" s="20"/>
-      <c r="N18" s="14"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="24"/>
       <c r="O18" s="17"/>
     </row>
-    <row r="19" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="21"/>
+    <row r="19" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="13"/>
       <c r="K19" s="1">
         <v>5</v>
       </c>
       <c r="L19" s="6">
         <v>45589</v>
       </c>
-      <c r="M19" s="20"/>
-      <c r="N19" s="14"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="24"/>
       <c r="O19" s="17"/>
     </row>
-    <row r="20" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="21"/>
+    <row r="20" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="13"/>
       <c r="K20" s="1">
         <v>6</v>
       </c>
       <c r="L20" s="11">
         <v>45590</v>
       </c>
-      <c r="M20" s="20"/>
-      <c r="N20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="25"/>
       <c r="O20" s="18"/>
     </row>
-    <row r="21" spans="7:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G21" s="21">
+    <row r="21" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G21" s="13">
         <v>2</v>
       </c>
-      <c r="H21" s="21" t="s">
+      <c r="H21" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="I21" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="J21" s="21">
+      <c r="I21" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="J21" s="13">
         <v>7</v>
       </c>
       <c r="K21" s="1">
@@ -1171,83 +1149,83 @@
       <c r="L21" s="6">
         <v>45593</v>
       </c>
-      <c r="M21" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="N21" s="13">
+      <c r="M21" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="N21" s="23">
         <v>15</v>
       </c>
       <c r="O21" s="16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="21"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="13"/>
       <c r="K22" s="1">
         <v>3</v>
       </c>
       <c r="L22" s="6">
         <v>45594</v>
       </c>
-      <c r="M22" s="20"/>
-      <c r="N22" s="14"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="24"/>
       <c r="O22" s="17"/>
     </row>
-    <row r="23" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="21"/>
+    <row r="23" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="13"/>
       <c r="K23" s="1">
         <v>4</v>
       </c>
       <c r="L23" s="6">
         <v>45595</v>
       </c>
-      <c r="M23" s="20"/>
-      <c r="N23" s="14"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="24"/>
       <c r="O23" s="17"/>
     </row>
-    <row r="24" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="21"/>
+    <row r="24" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="13"/>
       <c r="K24" s="1">
         <v>5</v>
       </c>
       <c r="L24" s="6">
         <v>45596</v>
       </c>
-      <c r="M24" s="20"/>
-      <c r="N24" s="14"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="24"/>
       <c r="O24" s="17"/>
     </row>
-    <row r="25" spans="7:15" ht="95.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="21"/>
+    <row r="25" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="13"/>
       <c r="K25" s="1">
         <v>6</v>
       </c>
       <c r="L25" s="12">
         <v>45597</v>
       </c>
-      <c r="M25" s="20"/>
-      <c r="N25" s="15"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="25"/>
       <c r="O25" s="18"/>
     </row>
-    <row r="26" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="J26" s="21">
+    <row r="26" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="J26" s="13">
         <v>8</v>
       </c>
       <c r="K26" s="1">
@@ -1256,87 +1234,87 @@
       <c r="L26" s="6">
         <v>45600</v>
       </c>
-      <c r="M26" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="N26" s="13">
+      <c r="M26" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="N26" s="23">
         <v>15</v>
       </c>
       <c r="O26" s="16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="20"/>
-      <c r="J27" s="21"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="13"/>
       <c r="K27" s="1">
         <v>3</v>
       </c>
       <c r="L27" s="6">
         <v>45601</v>
       </c>
-      <c r="M27" s="20"/>
-      <c r="N27" s="14"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="24"/>
       <c r="O27" s="17"/>
     </row>
-    <row r="28" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="20"/>
-      <c r="J28" s="21"/>
+    <row r="28" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="13"/>
       <c r="K28" s="1">
         <v>4</v>
       </c>
       <c r="L28" s="6">
         <v>45602</v>
       </c>
-      <c r="M28" s="20"/>
-      <c r="N28" s="14"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="24"/>
       <c r="O28" s="17"/>
     </row>
-    <row r="29" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="20"/>
-      <c r="J29" s="21"/>
+    <row r="29" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="13"/>
       <c r="K29" s="1">
         <v>5</v>
       </c>
       <c r="L29" s="6">
         <v>45603</v>
       </c>
-      <c r="M29" s="20"/>
-      <c r="N29" s="14"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="24"/>
       <c r="O29" s="17"/>
     </row>
-    <row r="30" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="21"/>
+    <row r="30" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="13"/>
       <c r="K30" s="1">
         <v>6</v>
       </c>
       <c r="L30" s="6">
         <v>45604</v>
       </c>
-      <c r="M30" s="20"/>
-      <c r="N30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="25"/>
       <c r="O30" s="18"/>
     </row>
-    <row r="31" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G31" s="21">
+    <row r="31" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G31" s="13">
         <v>3</v>
       </c>
-      <c r="H31" s="21" t="s">
+      <c r="H31" s="13" t="s">
         <v>10</v>
       </c>
       <c r="I31" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="J31" s="21">
+        <v>79</v>
+      </c>
+      <c r="J31" s="13">
         <v>9</v>
       </c>
       <c r="K31" s="1">
@@ -1346,20 +1324,20 @@
         <v>45607</v>
       </c>
       <c r="M31" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="N31" s="13">
+        <v>78</v>
+      </c>
+      <c r="N31" s="23">
         <v>15</v>
       </c>
       <c r="O31" s="16" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="32" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G32" s="21"/>
-      <c r="H32" s="21"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
       <c r="I32" s="17"/>
-      <c r="J32" s="21"/>
+      <c r="J32" s="13"/>
       <c r="K32" s="1">
         <v>3</v>
       </c>
@@ -1367,14 +1345,14 @@
         <v>45608</v>
       </c>
       <c r="M32" s="17"/>
-      <c r="N32" s="14"/>
+      <c r="N32" s="24"/>
       <c r="O32" s="17"/>
     </row>
-    <row r="33" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
+    <row r="33" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
       <c r="I33" s="17"/>
-      <c r="J33" s="21"/>
+      <c r="J33" s="13"/>
       <c r="K33" s="1">
         <v>4</v>
       </c>
@@ -1382,14 +1360,14 @@
         <v>45609</v>
       </c>
       <c r="M33" s="17"/>
-      <c r="N33" s="14"/>
+      <c r="N33" s="24"/>
       <c r="O33" s="17"/>
     </row>
-    <row r="34" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
+    <row r="34" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
       <c r="I34" s="17"/>
-      <c r="J34" s="21"/>
+      <c r="J34" s="13"/>
       <c r="K34" s="1">
         <v>5</v>
       </c>
@@ -1397,14 +1375,14 @@
         <v>45610</v>
       </c>
       <c r="M34" s="17"/>
-      <c r="N34" s="14"/>
+      <c r="N34" s="24"/>
       <c r="O34" s="17"/>
     </row>
-    <row r="35" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
+    <row r="35" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
       <c r="I35" s="18"/>
-      <c r="J35" s="21"/>
+      <c r="J35" s="13"/>
       <c r="K35" s="1">
         <v>6</v>
       </c>
@@ -1412,16 +1390,16 @@
         <v>45611</v>
       </c>
       <c r="M35" s="18"/>
-      <c r="N35" s="15"/>
+      <c r="N35" s="25"/>
       <c r="O35" s="18"/>
     </row>
-    <row r="36" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G36" s="21"/>
-      <c r="H36" s="21"/>
-      <c r="I36" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="J36" s="21">
+    <row r="36" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="J36" s="13">
         <v>10</v>
       </c>
       <c r="K36" s="1">
@@ -1430,87 +1408,87 @@
       <c r="L36" s="6">
         <v>45614</v>
       </c>
-      <c r="M36" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="N36" s="13">
+      <c r="M36" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="N36" s="23">
         <v>15</v>
       </c>
-      <c r="O36" s="13" t="s">
+      <c r="O36" s="23" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G37" s="21"/>
-      <c r="H37" s="21"/>
-      <c r="I37" s="20"/>
-      <c r="J37" s="21"/>
+    <row r="37" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="13"/>
       <c r="K37" s="1">
         <v>3</v>
       </c>
       <c r="L37" s="6">
         <v>45615</v>
       </c>
-      <c r="M37" s="20"/>
-      <c r="N37" s="14"/>
-      <c r="O37" s="14"/>
-    </row>
-    <row r="38" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G38" s="21"/>
-      <c r="H38" s="21"/>
-      <c r="I38" s="20"/>
-      <c r="J38" s="21"/>
+      <c r="M37" s="15"/>
+      <c r="N37" s="24"/>
+      <c r="O37" s="24"/>
+    </row>
+    <row r="38" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="13"/>
       <c r="K38" s="1">
         <v>4</v>
       </c>
       <c r="L38" s="6">
         <v>45616</v>
       </c>
-      <c r="M38" s="20"/>
-      <c r="N38" s="14"/>
-      <c r="O38" s="14"/>
-    </row>
-    <row r="39" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G39" s="21"/>
-      <c r="H39" s="21"/>
-      <c r="I39" s="20"/>
-      <c r="J39" s="21"/>
+      <c r="M38" s="15"/>
+      <c r="N38" s="24"/>
+      <c r="O38" s="24"/>
+    </row>
+    <row r="39" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="15"/>
+      <c r="J39" s="13"/>
       <c r="K39" s="1">
         <v>5</v>
       </c>
       <c r="L39" s="6">
         <v>45617</v>
       </c>
-      <c r="M39" s="20"/>
-      <c r="N39" s="14"/>
-      <c r="O39" s="14"/>
-    </row>
-    <row r="40" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G40" s="21"/>
-      <c r="H40" s="21"/>
-      <c r="I40" s="20"/>
-      <c r="J40" s="21"/>
+      <c r="M39" s="15"/>
+      <c r="N39" s="24"/>
+      <c r="O39" s="24"/>
+    </row>
+    <row r="40" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="13"/>
       <c r="K40" s="1">
         <v>6</v>
       </c>
       <c r="L40" s="6">
         <v>45618</v>
       </c>
-      <c r="M40" s="20"/>
-      <c r="N40" s="15"/>
-      <c r="O40" s="15"/>
-    </row>
-    <row r="41" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G41" s="21">
+      <c r="M40" s="15"/>
+      <c r="N40" s="25"/>
+      <c r="O40" s="25"/>
+    </row>
+    <row r="41" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G41" s="13">
         <v>4</v>
       </c>
-      <c r="H41" s="21" t="s">
+      <c r="H41" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I41" s="20" t="s">
+      <c r="I41" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="J41" s="21">
+      <c r="J41" s="13">
         <v>11</v>
       </c>
       <c r="K41" s="1">
@@ -1519,94 +1497,93 @@
       <c r="L41" s="6">
         <v>45621</v>
       </c>
-      <c r="M41" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="N41" s="13">
+      <c r="M41" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="N41" s="23">
         <v>15</v>
       </c>
-      <c r="O41" s="13" t="s">
+      <c r="O41" s="23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G42" s="21"/>
-      <c r="H42" s="21"/>
-      <c r="I42" s="20"/>
-      <c r="J42" s="21"/>
+    <row r="42" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="15"/>
+      <c r="J42" s="13"/>
       <c r="K42" s="1">
         <v>3</v>
       </c>
       <c r="L42" s="6">
         <v>45622</v>
       </c>
-      <c r="M42" s="20"/>
-      <c r="N42" s="14"/>
-      <c r="O42" s="14"/>
-    </row>
-    <row r="43" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G43" s="21"/>
-      <c r="H43" s="21"/>
-      <c r="I43" s="20"/>
-      <c r="J43" s="21"/>
+      <c r="M42" s="15"/>
+      <c r="N42" s="24"/>
+      <c r="O42" s="24"/>
+    </row>
+    <row r="43" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="15"/>
+      <c r="J43" s="13"/>
       <c r="K43" s="1">
         <v>4</v>
       </c>
       <c r="L43" s="6">
         <v>45623</v>
       </c>
-      <c r="M43" s="20"/>
-      <c r="N43" s="14"/>
-      <c r="O43" s="14"/>
-    </row>
-    <row r="44" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G44" s="21"/>
-      <c r="H44" s="21"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="21"/>
+      <c r="M43" s="15"/>
+      <c r="N43" s="24"/>
+      <c r="O43" s="24"/>
+    </row>
+    <row r="44" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="15"/>
+      <c r="J44" s="13"/>
       <c r="K44" s="1">
         <v>5</v>
       </c>
       <c r="L44" s="6">
         <v>45624</v>
       </c>
-      <c r="M44" s="20"/>
-      <c r="N44" s="14"/>
-      <c r="O44" s="14"/>
-    </row>
-    <row r="45" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G45" s="21"/>
-      <c r="H45" s="21"/>
-      <c r="I45" s="20"/>
-      <c r="J45" s="21"/>
+      <c r="M44" s="15"/>
+      <c r="N44" s="24"/>
+      <c r="O44" s="24"/>
+    </row>
+    <row r="45" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="15"/>
+      <c r="J45" s="13"/>
       <c r="K45" s="1">
         <v>6</v>
       </c>
       <c r="L45" s="6">
         <v>45625</v>
       </c>
-      <c r="M45" s="20"/>
-      <c r="N45" s="15"/>
-      <c r="O45" s="15"/>
+      <c r="M45" s="15"/>
+      <c r="N45" s="25"/>
+      <c r="O45" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="J31:J35"/>
-    <mergeCell ref="G21:G30"/>
-    <mergeCell ref="H21:H30"/>
-    <mergeCell ref="I21:I25"/>
-    <mergeCell ref="I26:I30"/>
-    <mergeCell ref="G31:G40"/>
-    <mergeCell ref="H31:H40"/>
-    <mergeCell ref="I36:I40"/>
-    <mergeCell ref="J26:J30"/>
-    <mergeCell ref="J21:J25"/>
-    <mergeCell ref="I31:I35"/>
-    <mergeCell ref="G41:G45"/>
-    <mergeCell ref="H41:H45"/>
-    <mergeCell ref="I41:I45"/>
-    <mergeCell ref="J41:J45"/>
-    <mergeCell ref="J36:J40"/>
+    <mergeCell ref="O41:O45"/>
+    <mergeCell ref="O36:O40"/>
+    <mergeCell ref="O31:O35"/>
+    <mergeCell ref="N31:N35"/>
+    <mergeCell ref="M31:M35"/>
+    <mergeCell ref="M36:M40"/>
+    <mergeCell ref="N36:N40"/>
+    <mergeCell ref="M41:M45"/>
+    <mergeCell ref="N41:N45"/>
+    <mergeCell ref="N21:N25"/>
+    <mergeCell ref="M21:M25"/>
+    <mergeCell ref="O21:O25"/>
+    <mergeCell ref="M26:M30"/>
+    <mergeCell ref="N26:N30"/>
+    <mergeCell ref="O26:O30"/>
     <mergeCell ref="J16:J20"/>
     <mergeCell ref="J11:J15"/>
     <mergeCell ref="G8:O8"/>
@@ -1620,21 +1597,22 @@
     <mergeCell ref="I11:I15"/>
     <mergeCell ref="I16:I20"/>
     <mergeCell ref="O16:O20"/>
-    <mergeCell ref="N21:N25"/>
-    <mergeCell ref="M21:M25"/>
-    <mergeCell ref="O21:O25"/>
-    <mergeCell ref="M26:M30"/>
-    <mergeCell ref="N26:N30"/>
-    <mergeCell ref="O26:O30"/>
-    <mergeCell ref="O41:O45"/>
-    <mergeCell ref="O36:O40"/>
-    <mergeCell ref="O31:O35"/>
-    <mergeCell ref="N31:N35"/>
-    <mergeCell ref="M31:M35"/>
-    <mergeCell ref="M36:M40"/>
-    <mergeCell ref="N36:N40"/>
-    <mergeCell ref="M41:M45"/>
-    <mergeCell ref="N41:N45"/>
+    <mergeCell ref="G41:G45"/>
+    <mergeCell ref="H41:H45"/>
+    <mergeCell ref="I41:I45"/>
+    <mergeCell ref="J41:J45"/>
+    <mergeCell ref="J36:J40"/>
+    <mergeCell ref="J31:J35"/>
+    <mergeCell ref="G21:G30"/>
+    <mergeCell ref="H21:H30"/>
+    <mergeCell ref="I21:I25"/>
+    <mergeCell ref="I26:I30"/>
+    <mergeCell ref="G31:G40"/>
+    <mergeCell ref="H31:H40"/>
+    <mergeCell ref="I36:I40"/>
+    <mergeCell ref="J26:J30"/>
+    <mergeCell ref="J21:J25"/>
+    <mergeCell ref="I31:I35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1642,40 +1620,40 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="G8:O45"/>
   <sheetViews>
-    <sheetView topLeftCell="D13" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26:O30"/>
+    <sheetView topLeftCell="K19" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="7" max="7" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="72.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="74.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="52.53125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.06640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="70.86328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.53125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="75.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="7:15" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="G8" s="22" t="s">
+    <row r="8" spans="7:15" ht="22.5" x14ac:dyDescent="0.6">
+      <c r="G8" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22"/>
-      <c r="O8" s="22"/>
-    </row>
-    <row r="10" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
+    </row>
+    <row r="10" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
       <c r="G10" s="2" t="s">
         <v>0</v>
       </c>
@@ -1704,17 +1682,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G11" s="21">
+    <row r="11" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G11" s="13">
         <v>1</v>
       </c>
-      <c r="H11" s="21" t="s">
+      <c r="H11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="I11" s="19" t="s">
+      <c r="I11" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="J11" s="21">
+      <c r="J11" s="13">
         <v>5</v>
       </c>
       <c r="K11" s="1">
@@ -1726,18 +1704,18 @@
       <c r="M11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="N11" s="13">
+      <c r="N11" s="23">
         <v>5</v>
       </c>
       <c r="O11" s="16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="21"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="13"/>
       <c r="K12" s="1">
         <v>3</v>
       </c>
@@ -1745,16 +1723,16 @@
         <v>45580</v>
       </c>
       <c r="M12" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="N12" s="14"/>
+        <v>34</v>
+      </c>
+      <c r="N12" s="24"/>
       <c r="O12" s="17"/>
     </row>
-    <row r="13" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="21"/>
+    <row r="13" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="13"/>
       <c r="K13" s="1">
         <v>4</v>
       </c>
@@ -1762,14 +1740,14 @@
         <v>45581</v>
       </c>
       <c r="M13" s="17"/>
-      <c r="N13" s="14"/>
+      <c r="N13" s="24"/>
       <c r="O13" s="17"/>
     </row>
-    <row r="14" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="21"/>
+    <row r="14" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="13"/>
       <c r="K14" s="1">
         <v>5</v>
       </c>
@@ -1779,14 +1757,14 @@
       <c r="M14" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="N14" s="14"/>
+      <c r="N14" s="24"/>
       <c r="O14" s="17"/>
     </row>
-    <row r="15" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="21"/>
+    <row r="15" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="13"/>
       <c r="K15" s="1">
         <v>6</v>
       </c>
@@ -1794,16 +1772,16 @@
         <v>45583</v>
       </c>
       <c r="M15" s="18"/>
-      <c r="N15" s="15"/>
+      <c r="N15" s="25"/>
       <c r="O15" s="18"/>
     </row>
-    <row r="16" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="J16" s="21">
+    <row r="16" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J16" s="13">
         <v>6</v>
       </c>
       <c r="K16" s="1">
@@ -1812,21 +1790,21 @@
       <c r="L16" s="6">
         <v>45586</v>
       </c>
-      <c r="M16" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="N16" s="13">
+      <c r="M16" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="N16" s="23">
         <v>5</v>
       </c>
       <c r="O16" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="21"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="13"/>
       <c r="K17" s="1">
         <v>3</v>
       </c>
@@ -1834,14 +1812,14 @@
         <v>45587</v>
       </c>
       <c r="M17" s="18"/>
-      <c r="N17" s="14"/>
+      <c r="N17" s="24"/>
       <c r="O17" s="17"/>
     </row>
-    <row r="18" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="21"/>
+    <row r="18" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="13"/>
       <c r="K18" s="1">
         <v>4</v>
       </c>
@@ -1849,31 +1827,31 @@
         <v>45588</v>
       </c>
       <c r="M18" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="N18" s="14"/>
+        <v>37</v>
+      </c>
+      <c r="N18" s="24"/>
       <c r="O18" s="17"/>
     </row>
-    <row r="19" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="21"/>
+    <row r="19" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="13"/>
       <c r="K19" s="1">
         <v>5</v>
       </c>
       <c r="L19" s="6">
         <v>45589</v>
       </c>
-      <c r="M19" s="28"/>
-      <c r="N19" s="14"/>
+      <c r="M19" s="26"/>
+      <c r="N19" s="24"/>
       <c r="O19" s="17"/>
     </row>
-    <row r="20" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="21"/>
+    <row r="20" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="13"/>
       <c r="K20" s="1">
         <v>6</v>
       </c>
@@ -1881,22 +1859,22 @@
         <v>45590</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="N20" s="15"/>
+        <v>38</v>
+      </c>
+      <c r="N20" s="25"/>
       <c r="O20" s="18"/>
     </row>
-    <row r="21" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G21" s="21">
+    <row r="21" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G21" s="13">
         <v>2</v>
       </c>
-      <c r="H21" s="21" t="s">
+      <c r="H21" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="I21" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="J21" s="21">
+      <c r="I21" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="J21" s="13">
         <v>7</v>
       </c>
       <c r="K21" s="1">
@@ -1905,70 +1883,68 @@
       <c r="L21" s="6">
         <v>45593</v>
       </c>
-      <c r="M21" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="N21" s="13">
+      <c r="M21" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="N21" s="23">
         <v>5</v>
       </c>
       <c r="O21" s="16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="21"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="13"/>
       <c r="K22" s="1">
         <v>3</v>
       </c>
       <c r="L22" s="6">
         <v>45594</v>
       </c>
-      <c r="M22" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="N22" s="14"/>
+      <c r="M22" s="27"/>
+      <c r="N22" s="24"/>
       <c r="O22" s="17"/>
     </row>
-    <row r="23" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="21"/>
+    <row r="23" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="13"/>
       <c r="K23" s="1">
         <v>4</v>
       </c>
       <c r="L23" s="6">
         <v>45595</v>
       </c>
-      <c r="M23" s="18"/>
-      <c r="N23" s="14"/>
+      <c r="M23" s="26"/>
+      <c r="N23" s="24"/>
       <c r="O23" s="17"/>
     </row>
-    <row r="24" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="21"/>
+    <row r="24" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="13"/>
       <c r="K24" s="1">
         <v>5</v>
       </c>
       <c r="L24" s="6">
         <v>45596</v>
       </c>
-      <c r="M24" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="N24" s="14"/>
+      <c r="M24" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="N24" s="24"/>
       <c r="O24" s="17"/>
     </row>
-    <row r="25" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="21"/>
+    <row r="25" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="13"/>
       <c r="K25" s="1">
         <v>6</v>
       </c>
@@ -1976,16 +1952,16 @@
         <v>45597</v>
       </c>
       <c r="M25" s="18"/>
-      <c r="N25" s="15"/>
+      <c r="N25" s="25"/>
       <c r="O25" s="18"/>
     </row>
-    <row r="26" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="J26" s="21">
+    <row r="26" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="J26" s="13">
         <v>8</v>
       </c>
       <c r="K26" s="1">
@@ -1995,20 +1971,20 @@
         <v>45600</v>
       </c>
       <c r="M26" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="N26" s="13">
+        <v>90</v>
+      </c>
+      <c r="N26" s="23">
         <v>5</v>
       </c>
       <c r="O26" s="16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="20"/>
-      <c r="J27" s="21"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="13"/>
       <c r="K27" s="1">
         <v>3</v>
       </c>
@@ -2016,46 +1992,46 @@
         <v>45601</v>
       </c>
       <c r="M27" s="27"/>
-      <c r="N27" s="14"/>
+      <c r="N27" s="24"/>
       <c r="O27" s="17"/>
     </row>
-    <row r="28" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="20"/>
-      <c r="J28" s="21"/>
+    <row r="28" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="13"/>
       <c r="K28" s="1">
         <v>4</v>
       </c>
       <c r="L28" s="6">
         <v>45602</v>
       </c>
-      <c r="M28" s="28"/>
-      <c r="N28" s="14"/>
+      <c r="M28" s="26"/>
+      <c r="N28" s="24"/>
       <c r="O28" s="17"/>
     </row>
-    <row r="29" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="20"/>
-      <c r="J29" s="21"/>
+    <row r="29" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="13"/>
       <c r="K29" s="1">
         <v>5</v>
       </c>
       <c r="L29" s="6">
         <v>45603</v>
       </c>
-      <c r="M29" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="N29" s="14"/>
+      <c r="M29" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="N29" s="24"/>
       <c r="O29" s="17"/>
     </row>
-    <row r="30" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="21"/>
+    <row r="30" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="13"/>
       <c r="K30" s="1">
         <v>6</v>
       </c>
@@ -2063,20 +2039,20 @@
         <v>45604</v>
       </c>
       <c r="M30" s="18"/>
-      <c r="N30" s="15"/>
+      <c r="N30" s="25"/>
       <c r="O30" s="18"/>
     </row>
-    <row r="31" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G31" s="21">
+    <row r="31" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G31" s="13">
         <v>3</v>
       </c>
-      <c r="H31" s="21" t="s">
+      <c r="H31" s="13" t="s">
         <v>10</v>
       </c>
       <c r="I31" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="J31" s="21">
+        <v>79</v>
+      </c>
+      <c r="J31" s="13">
         <v>9</v>
       </c>
       <c r="K31" s="1">
@@ -2086,20 +2062,20 @@
         <v>45607</v>
       </c>
       <c r="M31" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="N31" s="13">
-        <v>5</v>
-      </c>
-      <c r="O31" s="13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="32" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G32" s="21"/>
-      <c r="H32" s="21"/>
+        <v>92</v>
+      </c>
+      <c r="N31" s="23">
+        <v>5</v>
+      </c>
+      <c r="O31" s="16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
       <c r="I32" s="17"/>
-      <c r="J32" s="21"/>
+      <c r="J32" s="13"/>
       <c r="K32" s="1">
         <v>3</v>
       </c>
@@ -2107,14 +2083,14 @@
         <v>45608</v>
       </c>
       <c r="M32" s="17"/>
-      <c r="N32" s="14"/>
-      <c r="O32" s="14"/>
-    </row>
-    <row r="33" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
+      <c r="N32" s="24"/>
+      <c r="O32" s="17"/>
+    </row>
+    <row r="33" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
       <c r="I33" s="17"/>
-      <c r="J33" s="21"/>
+      <c r="J33" s="13"/>
       <c r="K33" s="1">
         <v>4</v>
       </c>
@@ -2122,14 +2098,14 @@
         <v>45609</v>
       </c>
       <c r="M33" s="17"/>
-      <c r="N33" s="14"/>
-      <c r="O33" s="14"/>
-    </row>
-    <row r="34" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
+      <c r="N33" s="24"/>
+      <c r="O33" s="17"/>
+    </row>
+    <row r="34" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
       <c r="I34" s="17"/>
-      <c r="J34" s="21"/>
+      <c r="J34" s="13"/>
       <c r="K34" s="1">
         <v>5</v>
       </c>
@@ -2137,14 +2113,14 @@
         <v>45610</v>
       </c>
       <c r="M34" s="17"/>
-      <c r="N34" s="14"/>
-      <c r="O34" s="14"/>
-    </row>
-    <row r="35" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
+      <c r="N34" s="24"/>
+      <c r="O34" s="17"/>
+    </row>
+    <row r="35" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
       <c r="I35" s="18"/>
-      <c r="J35" s="21"/>
+      <c r="J35" s="13"/>
       <c r="K35" s="1">
         <v>6</v>
       </c>
@@ -2152,16 +2128,16 @@
         <v>45611</v>
       </c>
       <c r="M35" s="18"/>
-      <c r="N35" s="15"/>
-      <c r="O35" s="15"/>
-    </row>
-    <row r="36" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G36" s="21"/>
-      <c r="H36" s="21"/>
-      <c r="I36" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="J36" s="21">
+      <c r="N35" s="25"/>
+      <c r="O35" s="18"/>
+    </row>
+    <row r="36" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="J36" s="13">
         <v>10</v>
       </c>
       <c r="K36" s="1">
@@ -2170,87 +2146,87 @@
       <c r="L36" s="6">
         <v>45614</v>
       </c>
-      <c r="M36" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="N36" s="13">
-        <v>5</v>
-      </c>
-      <c r="O36" s="13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="37" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G37" s="21"/>
-      <c r="H37" s="21"/>
-      <c r="I37" s="20"/>
-      <c r="J37" s="21"/>
+      <c r="M36" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="N36" s="23">
+        <v>5</v>
+      </c>
+      <c r="O36" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="13"/>
       <c r="K37" s="1">
         <v>3</v>
       </c>
       <c r="L37" s="6">
         <v>45615</v>
       </c>
-      <c r="M37" s="20"/>
-      <c r="N37" s="14"/>
-      <c r="O37" s="14"/>
-    </row>
-    <row r="38" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G38" s="21"/>
-      <c r="H38" s="21"/>
-      <c r="I38" s="20"/>
-      <c r="J38" s="21"/>
+      <c r="M37" s="15"/>
+      <c r="N37" s="24"/>
+      <c r="O37" s="24"/>
+    </row>
+    <row r="38" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="13"/>
       <c r="K38" s="1">
         <v>4</v>
       </c>
       <c r="L38" s="6">
         <v>45616</v>
       </c>
-      <c r="M38" s="20"/>
-      <c r="N38" s="14"/>
-      <c r="O38" s="14"/>
-    </row>
-    <row r="39" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G39" s="21"/>
-      <c r="H39" s="21"/>
-      <c r="I39" s="20"/>
-      <c r="J39" s="21"/>
+      <c r="M38" s="15"/>
+      <c r="N38" s="24"/>
+      <c r="O38" s="24"/>
+    </row>
+    <row r="39" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="15"/>
+      <c r="J39" s="13"/>
       <c r="K39" s="1">
         <v>5</v>
       </c>
       <c r="L39" s="6">
         <v>45617</v>
       </c>
-      <c r="M39" s="20"/>
-      <c r="N39" s="14"/>
-      <c r="O39" s="14"/>
-    </row>
-    <row r="40" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G40" s="21"/>
-      <c r="H40" s="21"/>
-      <c r="I40" s="20"/>
-      <c r="J40" s="21"/>
+      <c r="M39" s="15"/>
+      <c r="N39" s="24"/>
+      <c r="O39" s="24"/>
+    </row>
+    <row r="40" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="13"/>
       <c r="K40" s="1">
         <v>6</v>
       </c>
       <c r="L40" s="6">
         <v>45618</v>
       </c>
-      <c r="M40" s="20"/>
-      <c r="N40" s="15"/>
-      <c r="O40" s="15"/>
-    </row>
-    <row r="41" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G41" s="21">
+      <c r="M40" s="15"/>
+      <c r="N40" s="25"/>
+      <c r="O40" s="25"/>
+    </row>
+    <row r="41" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G41" s="13">
         <v>4</v>
       </c>
-      <c r="H41" s="21" t="s">
+      <c r="H41" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I41" s="20" t="s">
+      <c r="I41" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="J41" s="21">
+      <c r="J41" s="13">
         <v>11</v>
       </c>
       <c r="K41" s="1">
@@ -2259,102 +2235,86 @@
       <c r="L41" s="6">
         <v>45621</v>
       </c>
-      <c r="M41" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="N41" s="13">
-        <v>5</v>
-      </c>
-      <c r="O41" s="13" t="s">
+      <c r="M41" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="N41" s="23">
+        <v>5</v>
+      </c>
+      <c r="O41" s="23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G42" s="21"/>
-      <c r="H42" s="21"/>
-      <c r="I42" s="20"/>
-      <c r="J42" s="21"/>
+    <row r="42" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="15"/>
+      <c r="J42" s="13"/>
       <c r="K42" s="1">
         <v>3</v>
       </c>
       <c r="L42" s="6">
         <v>45622</v>
       </c>
-      <c r="M42" s="20"/>
-      <c r="N42" s="14"/>
-      <c r="O42" s="14"/>
-    </row>
-    <row r="43" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G43" s="21"/>
-      <c r="H43" s="21"/>
-      <c r="I43" s="20"/>
-      <c r="J43" s="21"/>
+      <c r="M42" s="15"/>
+      <c r="N42" s="24"/>
+      <c r="O42" s="24"/>
+    </row>
+    <row r="43" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="15"/>
+      <c r="J43" s="13"/>
       <c r="K43" s="1">
         <v>4</v>
       </c>
       <c r="L43" s="6">
         <v>45623</v>
       </c>
-      <c r="M43" s="20"/>
-      <c r="N43" s="14"/>
-      <c r="O43" s="14"/>
-    </row>
-    <row r="44" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G44" s="21"/>
-      <c r="H44" s="21"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="21"/>
+      <c r="M43" s="15"/>
+      <c r="N43" s="24"/>
+      <c r="O43" s="24"/>
+    </row>
+    <row r="44" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="15"/>
+      <c r="J44" s="13"/>
       <c r="K44" s="1">
         <v>5</v>
       </c>
       <c r="L44" s="6">
         <v>45624</v>
       </c>
-      <c r="M44" s="20"/>
-      <c r="N44" s="14"/>
-      <c r="O44" s="14"/>
-    </row>
-    <row r="45" spans="7:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="G45" s="21"/>
-      <c r="H45" s="21"/>
-      <c r="I45" s="20"/>
-      <c r="J45" s="21"/>
+      <c r="M44" s="15"/>
+      <c r="N44" s="24"/>
+      <c r="O44" s="24"/>
+    </row>
+    <row r="45" spans="7:15" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="15"/>
+      <c r="J45" s="13"/>
       <c r="K45" s="1">
         <v>6</v>
       </c>
       <c r="L45" s="6">
         <v>45625</v>
       </c>
-      <c r="M45" s="20"/>
-      <c r="N45" s="15"/>
-      <c r="O45" s="15"/>
+      <c r="M45" s="15"/>
+      <c r="N45" s="25"/>
+      <c r="O45" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="G8:O8"/>
-    <mergeCell ref="G11:G20"/>
-    <mergeCell ref="H11:H20"/>
-    <mergeCell ref="I11:I15"/>
-    <mergeCell ref="J11:J15"/>
-    <mergeCell ref="N11:N15"/>
-    <mergeCell ref="O11:O15"/>
-    <mergeCell ref="I16:I20"/>
-    <mergeCell ref="J16:J20"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="M12:M13"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="M36:M40"/>
-    <mergeCell ref="G21:G30"/>
-    <mergeCell ref="H21:H30"/>
-    <mergeCell ref="I21:I25"/>
-    <mergeCell ref="J21:J25"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="M26:M28"/>
-    <mergeCell ref="M29:M30"/>
-    <mergeCell ref="I26:I30"/>
-    <mergeCell ref="J26:J30"/>
+    <mergeCell ref="N31:N35"/>
+    <mergeCell ref="O31:O35"/>
+    <mergeCell ref="N16:N20"/>
+    <mergeCell ref="O16:O20"/>
+    <mergeCell ref="N21:N25"/>
+    <mergeCell ref="O21:O25"/>
+    <mergeCell ref="N26:N30"/>
+    <mergeCell ref="O26:O30"/>
     <mergeCell ref="N36:N40"/>
     <mergeCell ref="O36:O40"/>
     <mergeCell ref="G41:G45"/>
@@ -2371,14 +2331,30 @@
     <mergeCell ref="M31:M35"/>
     <mergeCell ref="I36:I40"/>
     <mergeCell ref="J36:J40"/>
-    <mergeCell ref="N31:N35"/>
-    <mergeCell ref="O31:O35"/>
-    <mergeCell ref="N16:N20"/>
-    <mergeCell ref="O16:O20"/>
-    <mergeCell ref="N21:N25"/>
-    <mergeCell ref="O21:O25"/>
-    <mergeCell ref="N26:N30"/>
-    <mergeCell ref="O26:O30"/>
+    <mergeCell ref="M36:M40"/>
+    <mergeCell ref="G21:G30"/>
+    <mergeCell ref="H21:H30"/>
+    <mergeCell ref="I21:I25"/>
+    <mergeCell ref="J21:J25"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="M26:M28"/>
+    <mergeCell ref="M29:M30"/>
+    <mergeCell ref="I26:I30"/>
+    <mergeCell ref="J26:J30"/>
+    <mergeCell ref="M21:M23"/>
+    <mergeCell ref="G8:O8"/>
+    <mergeCell ref="G11:G20"/>
+    <mergeCell ref="H11:H20"/>
+    <mergeCell ref="I11:I15"/>
+    <mergeCell ref="J11:J15"/>
+    <mergeCell ref="N11:N15"/>
+    <mergeCell ref="O11:O15"/>
+    <mergeCell ref="I16:I20"/>
+    <mergeCell ref="J16:J20"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="M16:M17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2386,27 +2362,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="C3:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19:K23"/>
+    <sheetView topLeftCell="B3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.3984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="51.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="39.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.06640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="50.06640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.53125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="39.06640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
@@ -2435,17 +2411,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C4" s="21">
+    <row r="4" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C4" s="13">
         <v>1</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="13">
         <v>5</v>
       </c>
       <c r="G4" s="1">
@@ -2457,84 +2433,84 @@
       <c r="I4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="23">
         <v>5</v>
       </c>
       <c r="K4" s="16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="21"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="13"/>
       <c r="G5" s="1">
         <v>3</v>
       </c>
       <c r="H5" s="10">
         <v>45580</v>
       </c>
-      <c r="I5" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="J5" s="14"/>
+      <c r="I5" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" s="24"/>
       <c r="K5" s="17"/>
     </row>
-    <row r="6" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="21"/>
+    <row r="6" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="13"/>
       <c r="G6" s="1">
         <v>4</v>
       </c>
       <c r="H6" s="10">
         <v>45581</v>
       </c>
-      <c r="I6" s="31"/>
-      <c r="J6" s="14"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="24"/>
       <c r="K6" s="17"/>
     </row>
-    <row r="7" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="21"/>
+    <row r="7" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="13"/>
       <c r="G7" s="1">
         <v>5</v>
       </c>
       <c r="H7" s="10">
         <v>45582</v>
       </c>
-      <c r="I7" s="31" t="s">
+      <c r="I7" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="J7" s="14"/>
+      <c r="J7" s="24"/>
       <c r="K7" s="17"/>
     </row>
-    <row r="8" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="21"/>
+    <row r="8" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="13"/>
       <c r="G8" s="1">
         <v>6</v>
       </c>
       <c r="H8" s="10">
         <v>45583</v>
       </c>
-      <c r="I8" s="32"/>
-      <c r="J8" s="15"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="25"/>
       <c r="K8" s="18"/>
     </row>
-    <row r="9" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="19" t="s">
+    <row r="9" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="21">
+      <c r="F9" s="13">
         <v>6</v>
       </c>
       <c r="G9" s="1">
@@ -2543,66 +2519,66 @@
       <c r="H9" s="10">
         <v>45586</v>
       </c>
-      <c r="I9" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="J9" s="13">
+      <c r="I9" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="J9" s="23">
         <v>5</v>
       </c>
       <c r="K9" s="16"/>
     </row>
-    <row r="10" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="21"/>
+    <row r="10" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="13"/>
       <c r="G10" s="1">
         <v>3</v>
       </c>
       <c r="H10" s="10">
         <v>45587</v>
       </c>
-      <c r="I10" s="32"/>
-      <c r="J10" s="14"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="24"/>
       <c r="K10" s="17"/>
     </row>
-    <row r="11" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="21"/>
+    <row r="11" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="13"/>
       <c r="G11" s="1">
         <v>4</v>
       </c>
       <c r="H11" s="10">
         <v>45588</v>
       </c>
-      <c r="I11" s="29" t="s">
+      <c r="I11" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="14"/>
+      <c r="J11" s="24"/>
       <c r="K11" s="17"/>
     </row>
-    <row r="12" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="21"/>
+    <row r="12" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="13"/>
       <c r="G12" s="1">
         <v>5</v>
       </c>
       <c r="H12" s="10">
         <v>45589</v>
       </c>
-      <c r="I12" s="30"/>
-      <c r="J12" s="14"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="24"/>
       <c r="K12" s="17"/>
     </row>
-    <row r="13" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="21"/>
+    <row r="13" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="13"/>
       <c r="G13" s="1">
         <v>6</v>
       </c>
@@ -2612,20 +2588,20 @@
       <c r="I13" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="J13" s="15"/>
+      <c r="J13" s="25"/>
       <c r="K13" s="18"/>
     </row>
-    <row r="14" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C14" s="21">
+    <row r="14" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C14" s="13">
         <v>2</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D14" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="F14" s="21">
+      <c r="E14" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="13">
         <v>7</v>
       </c>
       <c r="G14" s="1">
@@ -2634,85 +2610,85 @@
       <c r="H14" s="10">
         <v>45593</v>
       </c>
-      <c r="I14" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="J14" s="13">
+      <c r="I14" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="J14" s="23">
         <v>5</v>
       </c>
       <c r="K14" s="16" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="15" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="21"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="13"/>
       <c r="G15" s="1">
         <v>3</v>
       </c>
       <c r="H15" s="10">
         <v>45594</v>
       </c>
-      <c r="I15" s="35"/>
-      <c r="J15" s="14"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="24"/>
       <c r="K15" s="17"/>
     </row>
-    <row r="16" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="21"/>
+    <row r="16" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="13"/>
       <c r="G16" s="1">
         <v>4</v>
       </c>
       <c r="H16" s="10">
         <v>45595</v>
       </c>
-      <c r="I16" s="36"/>
-      <c r="J16" s="14"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="24"/>
       <c r="K16" s="17"/>
     </row>
-    <row r="17" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="21"/>
+    <row r="17" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="13"/>
       <c r="G17" s="1">
         <v>5</v>
       </c>
       <c r="H17" s="10">
         <v>45596</v>
       </c>
-      <c r="I17" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="J17" s="14"/>
+      <c r="I17" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="J17" s="24"/>
       <c r="K17" s="17"/>
     </row>
-    <row r="18" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="21"/>
+    <row r="18" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="13"/>
       <c r="G18" s="1">
         <v>6</v>
       </c>
       <c r="H18" s="10">
         <v>45597</v>
       </c>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="25"/>
       <c r="K18" s="18"/>
     </row>
-    <row r="19" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="F19" s="21">
+    <row r="19" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" s="13">
         <v>8</v>
       </c>
       <c r="G19" s="1">
@@ -2721,87 +2697,87 @@
       <c r="H19" s="10">
         <v>45600</v>
       </c>
-      <c r="I19" s="34" t="s">
-        <v>95</v>
-      </c>
-      <c r="J19" s="13">
+      <c r="I19" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="J19" s="23">
         <v>5</v>
       </c>
       <c r="K19" s="16"/>
     </row>
-    <row r="20" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="21"/>
+    <row r="20" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="13"/>
       <c r="G20" s="1">
         <v>3</v>
       </c>
       <c r="H20" s="10">
         <v>45601</v>
       </c>
-      <c r="I20" s="36"/>
-      <c r="J20" s="14"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="24"/>
       <c r="K20" s="17"/>
     </row>
-    <row r="21" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="21"/>
+    <row r="21" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="13"/>
       <c r="G21" s="1">
         <v>4</v>
       </c>
       <c r="H21" s="10">
         <v>45602</v>
       </c>
-      <c r="I21" s="13" t="s">
+      <c r="I21" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="J21" s="14"/>
+      <c r="J21" s="24"/>
       <c r="K21" s="17"/>
     </row>
-    <row r="22" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="21"/>
+    <row r="22" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="13"/>
       <c r="G22" s="1">
         <v>5</v>
       </c>
       <c r="H22" s="10">
         <v>45603</v>
       </c>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
       <c r="K22" s="17"/>
     </row>
-    <row r="23" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="21"/>
+    <row r="23" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="13"/>
       <c r="G23" s="1">
         <v>6</v>
       </c>
       <c r="H23" s="10">
         <v>45604</v>
       </c>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="25"/>
       <c r="K23" s="18"/>
     </row>
-    <row r="24" spans="3:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="21">
+    <row r="24" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C24" s="13">
         <v>3</v>
       </c>
-      <c r="D24" s="21" t="s">
+      <c r="D24" s="13" t="s">
         <v>10</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="F24" s="21">
+        <v>51</v>
+      </c>
+      <c r="F24" s="13">
         <v>9</v>
       </c>
       <c r="G24" s="1">
@@ -2810,85 +2786,85 @@
       <c r="H24" s="10">
         <v>45607</v>
       </c>
-      <c r="I24" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="J24" s="13">
-        <v>5</v>
-      </c>
-      <c r="K24" s="13" t="s">
+      <c r="I24" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="J24" s="23">
+        <v>5</v>
+      </c>
+      <c r="K24" s="23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
+    <row r="25" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
       <c r="E25" s="17"/>
-      <c r="F25" s="21"/>
+      <c r="F25" s="13"/>
       <c r="G25" s="1">
         <v>3</v>
       </c>
       <c r="H25" s="10">
         <v>45608</v>
       </c>
-      <c r="I25" s="36"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
-    </row>
-    <row r="26" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
+      <c r="I25" s="31"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24"/>
+    </row>
+    <row r="26" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
       <c r="E26" s="17"/>
-      <c r="F26" s="21"/>
+      <c r="F26" s="13"/>
       <c r="G26" s="1">
         <v>4</v>
       </c>
       <c r="H26" s="10">
         <v>45609</v>
       </c>
-      <c r="I26" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="J26" s="14"/>
-      <c r="K26" s="14"/>
-    </row>
-    <row r="27" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
+      <c r="I26" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
+    </row>
+    <row r="27" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
       <c r="E27" s="17"/>
-      <c r="F27" s="21"/>
+      <c r="F27" s="13"/>
       <c r="G27" s="1">
         <v>5</v>
       </c>
       <c r="H27" s="10">
         <v>45610</v>
       </c>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-    </row>
-    <row r="28" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
+      <c r="K27" s="24"/>
+    </row>
+    <row r="28" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
       <c r="E28" s="18"/>
-      <c r="F28" s="21"/>
+      <c r="F28" s="13"/>
       <c r="G28" s="1">
         <v>6</v>
       </c>
       <c r="H28" s="10">
         <v>45611</v>
       </c>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-    </row>
-    <row r="29" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="F29" s="21">
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
+      <c r="K28" s="25"/>
+    </row>
+    <row r="29" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29" s="13">
         <v>10</v>
       </c>
       <c r="G29" s="1">
@@ -2897,87 +2873,87 @@
       <c r="H29" s="10">
         <v>45614</v>
       </c>
-      <c r="I29" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="J29" s="13">
-        <v>5</v>
-      </c>
-      <c r="K29" s="13" t="s">
+      <c r="I29" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="J29" s="23">
+        <v>5</v>
+      </c>
+      <c r="K29" s="23" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="21"/>
+    <row r="30" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="13"/>
       <c r="G30" s="1">
         <v>3</v>
       </c>
       <c r="H30" s="10">
         <v>45615</v>
       </c>
-      <c r="I30" s="21"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="14"/>
-    </row>
-    <row r="31" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="21"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="24"/>
+    </row>
+    <row r="31" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="13"/>
       <c r="G31" s="1">
         <v>4</v>
       </c>
       <c r="H31" s="10">
         <v>45616</v>
       </c>
-      <c r="I31" s="21"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="14"/>
-    </row>
-    <row r="32" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="21"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="24"/>
+      <c r="K31" s="24"/>
+    </row>
+    <row r="32" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="13"/>
       <c r="G32" s="1">
         <v>5</v>
       </c>
       <c r="H32" s="10">
         <v>45617</v>
       </c>
-      <c r="I32" s="21"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="14"/>
-    </row>
-    <row r="33" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="21"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="24"/>
+      <c r="K32" s="24"/>
+    </row>
+    <row r="33" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="13"/>
       <c r="G33" s="1">
         <v>6</v>
       </c>
       <c r="H33" s="10">
         <v>45618</v>
       </c>
-      <c r="I33" s="21"/>
-      <c r="J33" s="15"/>
-      <c r="K33" s="15"/>
-    </row>
-    <row r="34" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C34" s="21">
+      <c r="I33" s="13"/>
+      <c r="J33" s="25"/>
+      <c r="K33" s="25"/>
+    </row>
+    <row r="34" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C34" s="13">
         <v>4</v>
       </c>
-      <c r="D34" s="21" t="s">
+      <c r="D34" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E34" s="20" t="s">
+      <c r="E34" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="F34" s="21">
+      <c r="F34" s="13">
         <v>11</v>
       </c>
       <c r="G34" s="1">
@@ -2986,88 +2962,100 @@
       <c r="H34" s="10">
         <v>45621</v>
       </c>
-      <c r="I34" s="19" t="s">
+      <c r="I34" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="J34" s="13">
-        <v>5</v>
-      </c>
-      <c r="K34" s="13" t="s">
+      <c r="J34" s="23">
+        <v>5</v>
+      </c>
+      <c r="K34" s="23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="21"/>
+    <row r="35" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="13"/>
       <c r="G35" s="1">
         <v>3</v>
       </c>
       <c r="H35" s="10">
         <v>45622</v>
       </c>
-      <c r="I35" s="20"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="14"/>
-    </row>
-    <row r="36" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C36" s="21"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="21"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="24"/>
+      <c r="K35" s="24"/>
+    </row>
+    <row r="36" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="13"/>
       <c r="G36" s="1">
         <v>4</v>
       </c>
       <c r="H36" s="10">
         <v>45623</v>
       </c>
-      <c r="I36" s="20"/>
-      <c r="J36" s="14"/>
-      <c r="K36" s="14"/>
-    </row>
-    <row r="37" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="21"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="24"/>
+      <c r="K36" s="24"/>
+    </row>
+    <row r="37" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="13"/>
       <c r="G37" s="1">
         <v>5</v>
       </c>
       <c r="H37" s="10">
         <v>45624</v>
       </c>
-      <c r="I37" s="20"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="14"/>
-    </row>
-    <row r="38" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="21"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="24"/>
+      <c r="K37" s="24"/>
+    </row>
+    <row r="38" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="13"/>
       <c r="G38" s="1">
         <v>6</v>
       </c>
       <c r="H38" s="10">
         <v>45625</v>
       </c>
-      <c r="I38" s="20"/>
-      <c r="J38" s="15"/>
-      <c r="K38" s="15"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="25"/>
+      <c r="K38" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="I14:I16"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="E9:E13"/>
-    <mergeCell ref="F9:F13"/>
-    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="K34:K38"/>
+    <mergeCell ref="C34:C38"/>
+    <mergeCell ref="D34:D38"/>
+    <mergeCell ref="E34:E38"/>
+    <mergeCell ref="F34:F38"/>
+    <mergeCell ref="I34:I38"/>
+    <mergeCell ref="J34:J38"/>
+    <mergeCell ref="F19:F23"/>
+    <mergeCell ref="J19:J23"/>
+    <mergeCell ref="K19:K23"/>
+    <mergeCell ref="C24:C33"/>
+    <mergeCell ref="D24:D33"/>
+    <mergeCell ref="E24:E28"/>
+    <mergeCell ref="F24:F28"/>
+    <mergeCell ref="I26:I28"/>
+    <mergeCell ref="K24:K28"/>
+    <mergeCell ref="E29:E33"/>
+    <mergeCell ref="F29:F33"/>
+    <mergeCell ref="I29:I33"/>
+    <mergeCell ref="J29:J33"/>
+    <mergeCell ref="K29:K33"/>
+    <mergeCell ref="J24:J28"/>
     <mergeCell ref="J9:J13"/>
     <mergeCell ref="K9:K13"/>
     <mergeCell ref="I11:I12"/>
@@ -3084,55 +3072,43 @@
     <mergeCell ref="K4:K8"/>
     <mergeCell ref="K14:K18"/>
     <mergeCell ref="E19:E23"/>
-    <mergeCell ref="F19:F23"/>
-    <mergeCell ref="J19:J23"/>
-    <mergeCell ref="K19:K23"/>
-    <mergeCell ref="C24:C33"/>
-    <mergeCell ref="D24:D33"/>
-    <mergeCell ref="E24:E28"/>
-    <mergeCell ref="F24:F28"/>
-    <mergeCell ref="I26:I28"/>
-    <mergeCell ref="K24:K28"/>
-    <mergeCell ref="E29:E33"/>
-    <mergeCell ref="F29:F33"/>
-    <mergeCell ref="I29:I33"/>
-    <mergeCell ref="J29:J33"/>
-    <mergeCell ref="K29:K33"/>
-    <mergeCell ref="J24:J28"/>
-    <mergeCell ref="K34:K38"/>
-    <mergeCell ref="C34:C38"/>
-    <mergeCell ref="D34:D38"/>
-    <mergeCell ref="E34:E38"/>
-    <mergeCell ref="F34:F38"/>
-    <mergeCell ref="I34:I38"/>
-    <mergeCell ref="J34:J38"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="E9:E13"/>
+    <mergeCell ref="F9:F13"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I14:I16"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="I24:I25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="C5:K36"/>
   <sheetViews>
-    <sheetView topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.3984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.06640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="46.3984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.53125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="99.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
       <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
@@ -3161,17 +3137,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="3:11" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="21">
+    <row r="6" spans="3:11" ht="33" x14ac:dyDescent="0.45">
+      <c r="C6" s="13">
         <v>1</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="13" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="13">
         <v>5</v>
       </c>
       <c r="G6" s="10">
@@ -3181,20 +3157,20 @@
         <v>2</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="J6" s="13">
+        <v>53</v>
+      </c>
+      <c r="J6" s="23">
         <v>15</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
       <c r="E7" s="27"/>
-      <c r="F7" s="21"/>
+      <c r="F7" s="13"/>
       <c r="G7" s="10">
         <v>45580</v>
       </c>
@@ -3202,16 +3178,16 @@
         <v>3</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="J7" s="14"/>
+        <v>54</v>
+      </c>
+      <c r="J7" s="24"/>
       <c r="K7" s="17"/>
     </row>
-    <row r="8" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
+    <row r="8" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
       <c r="E8" s="27"/>
-      <c r="F8" s="21"/>
+      <c r="F8" s="13"/>
       <c r="G8" s="10">
         <v>45581</v>
       </c>
@@ -3221,14 +3197,14 @@
       <c r="I8" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J8" s="14"/>
+      <c r="J8" s="24"/>
       <c r="K8" s="17"/>
     </row>
-    <row r="9" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="21"/>
+    <row r="9" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="13"/>
       <c r="G9" s="10">
         <v>45582</v>
       </c>
@@ -3238,16 +3214,16 @@
       <c r="I9" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="J9" s="14"/>
+      <c r="J9" s="24"/>
       <c r="K9" s="17"/>
     </row>
-    <row r="10" spans="3:11" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
+    <row r="10" spans="3:11" ht="33" x14ac:dyDescent="0.45">
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
       <c r="E10" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="21">
+      <c r="F10" s="13">
         <v>6</v>
       </c>
       <c r="G10" s="10">
@@ -3257,20 +3233,20 @@
         <v>2</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="J10" s="13">
+        <v>56</v>
+      </c>
+      <c r="J10" s="23">
         <v>15</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="3:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
       <c r="E11" s="27"/>
-      <c r="F11" s="21"/>
+      <c r="F11" s="13"/>
       <c r="G11" s="10">
         <v>45587</v>
       </c>
@@ -3278,16 +3254,16 @@
         <v>3</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="J11" s="14"/>
+        <v>57</v>
+      </c>
+      <c r="J11" s="24"/>
       <c r="K11" s="17"/>
     </row>
-    <row r="12" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
+    <row r="12" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
       <c r="E12" s="27"/>
-      <c r="F12" s="21"/>
+      <c r="F12" s="13"/>
       <c r="G12" s="10">
         <v>45588</v>
       </c>
@@ -3295,16 +3271,16 @@
         <v>4</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="J12" s="14"/>
+        <v>58</v>
+      </c>
+      <c r="J12" s="24"/>
       <c r="K12" s="17"/>
     </row>
-    <row r="13" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="21"/>
+    <row r="13" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="13"/>
       <c r="G13" s="10">
         <v>45589</v>
       </c>
@@ -3312,22 +3288,22 @@
         <v>5</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="J13" s="14"/>
+        <v>59</v>
+      </c>
+      <c r="J13" s="24"/>
       <c r="K13" s="17"/>
     </row>
-    <row r="14" spans="3:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="21">
+    <row r="14" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C14" s="13">
         <v>2</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D14" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="F14" s="21">
+      <c r="E14" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="13">
         <v>7</v>
       </c>
       <c r="G14" s="10">
@@ -3337,20 +3313,20 @@
         <v>2</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="J14" s="13">
+        <v>60</v>
+      </c>
+      <c r="J14" s="23">
         <v>15</v>
       </c>
       <c r="K14" s="16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="21"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="13"/>
       <c r="G15" s="10">
         <v>45594</v>
       </c>
@@ -3358,16 +3334,16 @@
         <v>3</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="J15" s="14"/>
+        <v>65</v>
+      </c>
+      <c r="J15" s="24"/>
       <c r="K15" s="17"/>
     </row>
-    <row r="16" spans="3:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="21"/>
+    <row r="16" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="13"/>
       <c r="G16" s="10">
         <v>45595</v>
       </c>
@@ -3375,18 +3351,18 @@
         <v>4</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="J16" s="14"/>
+        <v>61</v>
+      </c>
+      <c r="J16" s="24"/>
       <c r="K16" s="17"/>
     </row>
-    <row r="17" spans="3:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="F17" s="21">
+    <row r="17" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" s="13">
         <v>8</v>
       </c>
       <c r="G17" s="10">
@@ -3395,87 +3371,87 @@
       <c r="H17" s="1">
         <v>2</v>
       </c>
-      <c r="I17" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="J17" s="13">
+      <c r="I17" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="J17" s="23">
         <v>15</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="21"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="13"/>
       <c r="G18" s="10">
         <v>45601</v>
       </c>
       <c r="H18" s="1">
         <v>3</v>
       </c>
-      <c r="I18" s="20"/>
-      <c r="J18" s="14"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="24"/>
       <c r="K18" s="17"/>
     </row>
-    <row r="19" spans="3:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="21"/>
+    <row r="19" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="13"/>
       <c r="G19" s="10">
         <v>45602</v>
       </c>
       <c r="H19" s="1">
         <v>4</v>
       </c>
-      <c r="I19" s="20"/>
-      <c r="J19" s="14"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="24"/>
       <c r="K19" s="17"/>
     </row>
-    <row r="20" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="21"/>
+    <row r="20" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="13"/>
       <c r="G20" s="10">
         <v>45603</v>
       </c>
       <c r="H20" s="1">
         <v>5</v>
       </c>
-      <c r="I20" s="20"/>
-      <c r="J20" s="14"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="24"/>
       <c r="K20" s="17"/>
     </row>
-    <row r="21" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="21"/>
+    <row r="21" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="13"/>
       <c r="G21" s="10">
         <v>45604</v>
       </c>
       <c r="H21" s="1">
         <v>6</v>
       </c>
-      <c r="I21" s="20"/>
-      <c r="J21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="25"/>
       <c r="K21" s="18"/>
     </row>
-    <row r="22" spans="3:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="21">
+    <row r="22" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C22" s="13">
         <v>3</v>
       </c>
-      <c r="D22" s="21" t="s">
+      <c r="D22" s="13" t="s">
         <v>10</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="F22" s="21">
+        <v>51</v>
+      </c>
+      <c r="F22" s="13">
         <v>9</v>
       </c>
       <c r="G22" s="10">
@@ -3485,20 +3461,20 @@
         <v>2</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="J22" s="13">
+        <v>72</v>
+      </c>
+      <c r="J22" s="23">
         <v>15</v>
       </c>
-      <c r="K22" s="13" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
+      <c r="K22" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
       <c r="E23" s="27"/>
-      <c r="F23" s="21"/>
+      <c r="F23" s="13"/>
       <c r="G23" s="10">
         <v>45608</v>
       </c>
@@ -3506,33 +3482,33 @@
         <v>3</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-    </row>
-    <row r="24" spans="3:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
+        <v>73</v>
+      </c>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+    </row>
+    <row r="24" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
       <c r="E24" s="27"/>
-      <c r="F24" s="21"/>
+      <c r="F24" s="13"/>
       <c r="G24" s="10">
         <v>45609</v>
       </c>
       <c r="H24" s="1">
         <v>4</v>
       </c>
-      <c r="I24" s="26" t="s">
-        <v>94</v>
-      </c>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-    </row>
-    <row r="25" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
+      <c r="I24" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+    </row>
+    <row r="25" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
       <c r="E25" s="27"/>
-      <c r="F25" s="21"/>
+      <c r="F25" s="13"/>
       <c r="G25" s="10">
         <v>45610</v>
       </c>
@@ -3540,14 +3516,14 @@
         <v>5</v>
       </c>
       <c r="I25" s="17"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
-    </row>
-    <row r="26" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="21"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24"/>
+    </row>
+    <row r="26" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="13"/>
       <c r="G26" s="10">
         <v>45611</v>
       </c>
@@ -3555,16 +3531,16 @@
         <v>6</v>
       </c>
       <c r="I26" s="18"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-    </row>
-    <row r="27" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="25"/>
+    </row>
+    <row r="27" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
       <c r="E27" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="F27" s="21">
+        <v>63</v>
+      </c>
+      <c r="F27" s="13">
         <v>10</v>
       </c>
       <c r="G27" s="10">
@@ -3573,87 +3549,87 @@
       <c r="H27" s="1">
         <v>2</v>
       </c>
-      <c r="I27" s="20" t="s">
+      <c r="I27" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="J27" s="13">
+      <c r="J27" s="23">
         <v>15</v>
       </c>
-      <c r="K27" s="13" t="s">
+      <c r="K27" s="23" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
+    <row r="28" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
       <c r="E28" s="17"/>
-      <c r="F28" s="21"/>
+      <c r="F28" s="13"/>
       <c r="G28" s="10">
         <v>45615</v>
       </c>
       <c r="H28" s="1">
         <v>3</v>
       </c>
-      <c r="I28" s="20"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14"/>
-    </row>
-    <row r="29" spans="3:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="24"/>
+    </row>
+    <row r="29" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
       <c r="E29" s="17"/>
-      <c r="F29" s="21"/>
+      <c r="F29" s="13"/>
       <c r="G29" s="10">
         <v>45616</v>
       </c>
       <c r="H29" s="1">
         <v>4</v>
       </c>
-      <c r="I29" s="20"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="14"/>
-    </row>
-    <row r="30" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="24"/>
+      <c r="K29" s="24"/>
+    </row>
+    <row r="30" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
       <c r="E30" s="17"/>
-      <c r="F30" s="21"/>
+      <c r="F30" s="13"/>
       <c r="G30" s="10">
         <v>45617</v>
       </c>
       <c r="H30" s="1">
         <v>5</v>
       </c>
-      <c r="I30" s="20"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="14"/>
-    </row>
-    <row r="31" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="24"/>
+    </row>
+    <row r="31" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
       <c r="E31" s="18"/>
-      <c r="F31" s="21"/>
+      <c r="F31" s="13"/>
       <c r="G31" s="10">
         <v>45618</v>
       </c>
       <c r="H31" s="1">
         <v>6</v>
       </c>
-      <c r="I31" s="20"/>
-      <c r="J31" s="15"/>
-      <c r="K31" s="15"/>
-    </row>
-    <row r="32" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C32" s="21">
+      <c r="I31" s="15"/>
+      <c r="J31" s="25"/>
+      <c r="K31" s="25"/>
+    </row>
+    <row r="32" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C32" s="13">
         <v>4</v>
       </c>
-      <c r="D32" s="21" t="s">
+      <c r="D32" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E32" s="26" t="s">
+      <c r="E32" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="F32" s="21">
+      <c r="F32" s="13">
         <v>11</v>
       </c>
       <c r="G32" s="10">
@@ -3662,95 +3638,92 @@
       <c r="H32" s="1">
         <v>2</v>
       </c>
-      <c r="I32" s="19" t="s">
+      <c r="I32" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="J32" s="13">
+      <c r="J32" s="23">
         <v>15</v>
       </c>
-      <c r="K32" s="13" t="s">
+      <c r="K32" s="23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
+    <row r="33" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
       <c r="E33" s="17"/>
-      <c r="F33" s="21"/>
+      <c r="F33" s="13"/>
       <c r="G33" s="10">
         <v>45622</v>
       </c>
       <c r="H33" s="1">
         <v>3</v>
       </c>
-      <c r="I33" s="20"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="14"/>
-    </row>
-    <row r="34" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="24"/>
+      <c r="K33" s="24"/>
+    </row>
+    <row r="34" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
       <c r="E34" s="17"/>
-      <c r="F34" s="21"/>
+      <c r="F34" s="13"/>
       <c r="G34" s="10">
         <v>45623</v>
       </c>
       <c r="H34" s="1">
         <v>4</v>
       </c>
-      <c r="I34" s="20"/>
-      <c r="J34" s="14"/>
-      <c r="K34" s="14"/>
-    </row>
-    <row r="35" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="24"/>
+      <c r="K34" s="24"/>
+    </row>
+    <row r="35" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
       <c r="E35" s="17"/>
-      <c r="F35" s="21"/>
+      <c r="F35" s="13"/>
       <c r="G35" s="10">
         <v>45624</v>
       </c>
       <c r="H35" s="1">
         <v>5</v>
       </c>
-      <c r="I35" s="20"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="14"/>
-    </row>
-    <row r="36" spans="3:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C36" s="21"/>
-      <c r="D36" s="21"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="24"/>
+      <c r="K35" s="24"/>
+    </row>
+    <row r="36" spans="3:11" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
       <c r="E36" s="18"/>
-      <c r="F36" s="21"/>
+      <c r="F36" s="13"/>
       <c r="G36" s="10">
         <v>45625</v>
       </c>
       <c r="H36" s="1">
         <v>6</v>
       </c>
-      <c r="I36" s="20"/>
-      <c r="J36" s="15"/>
-      <c r="K36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="25"/>
+      <c r="K36" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="J6:J9"/>
-    <mergeCell ref="K6:K9"/>
-    <mergeCell ref="F10:F13"/>
-    <mergeCell ref="J10:J13"/>
-    <mergeCell ref="K10:K13"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="C6:C13"/>
-    <mergeCell ref="D6:D13"/>
-    <mergeCell ref="E6:E9"/>
-    <mergeCell ref="F6:F9"/>
-    <mergeCell ref="K14:K16"/>
-    <mergeCell ref="F17:F21"/>
-    <mergeCell ref="I17:I21"/>
-    <mergeCell ref="J17:J21"/>
-    <mergeCell ref="K17:K21"/>
-    <mergeCell ref="J14:J16"/>
-    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="K32:K36"/>
+    <mergeCell ref="C32:C36"/>
+    <mergeCell ref="D32:D36"/>
+    <mergeCell ref="E32:E36"/>
+    <mergeCell ref="F32:F36"/>
+    <mergeCell ref="I32:I36"/>
+    <mergeCell ref="J32:J36"/>
+    <mergeCell ref="K22:K26"/>
+    <mergeCell ref="E27:E31"/>
+    <mergeCell ref="F27:F31"/>
+    <mergeCell ref="I27:I31"/>
+    <mergeCell ref="J27:J31"/>
+    <mergeCell ref="K27:K31"/>
+    <mergeCell ref="J22:J26"/>
     <mergeCell ref="E17:E21"/>
     <mergeCell ref="I24:I26"/>
     <mergeCell ref="C22:C31"/>
@@ -3760,20 +3733,23 @@
     <mergeCell ref="C14:C21"/>
     <mergeCell ref="D14:D21"/>
     <mergeCell ref="E14:E16"/>
-    <mergeCell ref="K22:K26"/>
-    <mergeCell ref="E27:E31"/>
-    <mergeCell ref="F27:F31"/>
-    <mergeCell ref="I27:I31"/>
-    <mergeCell ref="J27:J31"/>
-    <mergeCell ref="K27:K31"/>
-    <mergeCell ref="J22:J26"/>
-    <mergeCell ref="K32:K36"/>
-    <mergeCell ref="C32:C36"/>
-    <mergeCell ref="D32:D36"/>
-    <mergeCell ref="E32:E36"/>
-    <mergeCell ref="F32:F36"/>
-    <mergeCell ref="I32:I36"/>
-    <mergeCell ref="J32:J36"/>
+    <mergeCell ref="K14:K16"/>
+    <mergeCell ref="F17:F21"/>
+    <mergeCell ref="I17:I21"/>
+    <mergeCell ref="J17:J21"/>
+    <mergeCell ref="K17:K21"/>
+    <mergeCell ref="J14:J16"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="C6:C13"/>
+    <mergeCell ref="D6:D13"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="F6:F9"/>
+    <mergeCell ref="J6:J9"/>
+    <mergeCell ref="K6:K9"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="J10:J13"/>
+    <mergeCell ref="K10:K13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>